<commit_message>
Started on organizing SATA and PCI
</commit_message>
<xml_diff>
--- a/Excel Sheet/Southbridge.xlsx
+++ b/Excel Sheet/Southbridge.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="90" windowWidth="20520" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="90" windowWidth="20520" windowHeight="11640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="balldiagram" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1702" uniqueCount="1042">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1913" uniqueCount="1050">
   <si>
     <t>A</t>
   </si>
@@ -3142,13 +3142,37 @@
   </si>
   <si>
     <t>REQ2# /GPIO52</t>
+  </si>
+  <si>
+    <t>clk</t>
+  </si>
+  <si>
+    <t>Data/ receive</t>
+  </si>
+  <si>
+    <t>Misc/Pwr</t>
+  </si>
+  <si>
+    <t>Unused</t>
+  </si>
+  <si>
+    <t>Serial ATA</t>
+  </si>
+  <si>
+    <t>Address Bus</t>
+  </si>
+  <si>
+    <t>command/enable</t>
+  </si>
+  <si>
+    <t>PCI Interface</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3186,8 +3210,31 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -3209,6 +3256,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3344,7 +3397,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3405,6 +3458,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5635,10 +5702,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B677"/>
+  <dimension ref="A1:D677"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A659" sqref="A659:B677"/>
+    <sheetView topLeftCell="A230" workbookViewId="0">
+      <selection activeCell="C240" sqref="C240:D240"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5646,7 +5713,7 @@
     <col min="1" max="1" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19.5" thickBot="1">
+    <row r="1" spans="1:4" ht="19.5" thickBot="1">
       <c r="A1" s="6" t="s">
         <v>120</v>
       </c>
@@ -5654,7 +5721,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" thickBot="1">
+    <row r="2" spans="1:4" ht="15.75" thickBot="1">
       <c r="A2" s="7" t="s">
         <v>122</v>
       </c>
@@ -5662,7 +5729,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" thickBot="1">
+    <row r="3" spans="1:4" ht="15.75" thickBot="1">
       <c r="A3" s="9" t="s">
         <v>124</v>
       </c>
@@ -5670,295 +5737,295 @@
         <v>125</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A4" s="9" t="s">
+    <row r="4" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C4" s="9" t="s">
         <v>126</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="D4" s="10" t="s">
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A5" s="9" t="s">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C5" s="9" t="s">
         <v>128</v>
       </c>
-      <c r="B5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A6" s="9" t="s">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C6" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="B6" s="10" t="s">
+      <c r="D6" s="10" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A7" s="9" t="s">
+    <row r="7" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C7" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B7" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A8" s="9" t="s">
+    <row r="8" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C8" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A9" s="9" t="s">
+    <row r="9" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C9" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="D9" s="10" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A10" s="9" t="s">
+    <row r="10" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C10" s="9" t="s">
         <v>137</v>
       </c>
-      <c r="B10" s="10" t="s">
+      <c r="D10" s="10" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A11" s="9" t="s">
+    <row r="11" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C11" s="9" t="s">
         <v>139</v>
       </c>
-      <c r="B11" s="10" t="s">
+      <c r="D11" s="10" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A12" s="9" t="s">
+    <row r="12" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C12" s="9" t="s">
         <v>141</v>
       </c>
-      <c r="B12" s="10" t="s">
+      <c r="D12" s="10" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A13" s="9" t="s">
+    <row r="13" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C13" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B13" s="10" t="s">
+      <c r="D13" s="10" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A14" s="9" t="s">
+    <row r="14" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C14" s="9" t="s">
         <v>144</v>
       </c>
-      <c r="B14" s="10" t="s">
+      <c r="D14" s="10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="15" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A15" s="9" t="s">
+    <row r="15" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C15" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="B15" s="10" t="s">
+      <c r="D15" s="10" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A16" s="9" t="s">
+    <row r="16" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C16" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="B16" s="10" t="s">
+      <c r="D16" s="10" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A17" s="9" t="s">
+    <row r="17" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C17" s="9" t="s">
         <v>149</v>
       </c>
-      <c r="B17" s="10" t="s">
+      <c r="D17" s="10" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A18" s="9" t="s">
+    <row r="18" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C18" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="D18" s="10" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A19" s="9" t="s">
+    <row r="19" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C19" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="B19" s="10" t="s">
+      <c r="D19" s="10" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C20" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="D20" s="10" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A21" s="9" t="s">
+    <row r="21" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C21" s="9" t="s">
         <v>154</v>
       </c>
-      <c r="B21" s="10" t="s">
+      <c r="D21" s="10" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A22" s="9" t="s">
+    <row r="22" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C22" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B22" s="10" t="s">
+      <c r="D22" s="10" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A23" s="9" t="s">
+    <row r="23" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C23" s="9" t="s">
         <v>158</v>
       </c>
-      <c r="B23" s="10" t="s">
+      <c r="D23" s="10" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A24" s="9" t="s">
+    <row r="24" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C24" s="9" t="s">
         <v>160</v>
       </c>
-      <c r="B24" s="10" t="s">
+      <c r="D24" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A25" s="9" t="s">
+    <row r="25" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C25" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B25" s="10" t="s">
+      <c r="D25" s="10" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A26" s="9" t="s">
+    <row r="26" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C26" s="9" t="s">
         <v>163</v>
       </c>
-      <c r="B26" s="10" t="s">
+      <c r="D26" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A27" s="9" t="s">
+    <row r="27" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C27" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="B27" s="10" t="s">
+      <c r="D27" s="10" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="28" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A28" s="9" t="s">
+    <row r="28" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C28" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B28" s="10" t="s">
+      <c r="D28" s="10" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A29" s="9" t="s">
+    <row r="29" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C29" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="10" t="s">
+      <c r="D29" s="10" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A30" s="9" t="s">
+    <row r="30" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C30" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="10" t="s">
+      <c r="D30" s="10" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="31" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A31" s="9" t="s">
+    <row r="31" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C31" s="9" t="s">
         <v>33</v>
       </c>
-      <c r="B31" s="10" t="s">
+      <c r="D31" s="10" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="32" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A32" s="9" t="s">
+    <row r="32" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C32" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="B32" s="10" t="s">
+      <c r="D32" s="10" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A33" s="9" t="s">
+    <row r="33" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C33" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B33" s="10" t="s">
+      <c r="D33" s="10" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A34" s="9" t="s">
+    <row r="34" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C34" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="10" t="s">
+      <c r="D34" s="10" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A35" s="9" t="s">
+    <row r="35" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C35" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B35" s="10" t="s">
+      <c r="D35" s="10" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A36" s="9" t="s">
+    <row r="36" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C36" s="9" t="s">
         <v>175</v>
       </c>
-      <c r="B36" s="10" t="s">
+      <c r="D36" s="10" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A37" s="9" t="s">
+    <row r="37" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C37" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="D37" s="10" t="s">
         <v>178</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A38" s="9" t="s">
+    <row r="38" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C38" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B38" s="10" t="s">
+      <c r="D38" s="10" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A39" s="9" t="s">
+    <row r="39" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C39" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="B39" s="10" t="s">
+      <c r="D39" s="10" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="21.75" thickBot="1">
+    <row r="40" spans="1:4" ht="15.75" thickBot="1">
       <c r="A40" s="9" t="s">
         <v>182</v>
       </c>
@@ -5966,7 +6033,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15.75" thickBot="1">
+    <row r="41" spans="1:4" ht="15.75" thickBot="1">
       <c r="A41" s="7" t="s">
         <v>184</v>
       </c>
@@ -5974,7 +6041,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="21.75" thickBot="1">
+    <row r="42" spans="1:4" ht="15.75" thickBot="1">
       <c r="A42" s="9" t="s">
         <v>186</v>
       </c>
@@ -5982,7 +6049,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="21.75" thickBot="1">
+    <row r="43" spans="1:4" ht="15.75" thickBot="1">
       <c r="A43" s="9" t="s">
         <v>188</v>
       </c>
@@ -5990,7 +6057,7 @@
         <v>189</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="21.75" thickBot="1">
+    <row r="44" spans="1:4" ht="15.75" thickBot="1">
       <c r="A44" s="9" t="s">
         <v>190</v>
       </c>
@@ -5998,7 +6065,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="15.75" thickBot="1">
+    <row r="45" spans="1:4" ht="15.75" thickBot="1">
       <c r="A45" s="9" t="s">
         <v>110</v>
       </c>
@@ -6006,7 +6073,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="15.75" thickBot="1">
+    <row r="46" spans="1:4" ht="15.75" thickBot="1">
       <c r="A46" s="9" t="s">
         <v>99</v>
       </c>
@@ -6014,7 +6081,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="21.75" thickBot="1">
+    <row r="47" spans="1:4" ht="15.75" thickBot="1">
       <c r="A47" s="9" t="s">
         <v>194</v>
       </c>
@@ -6022,7 +6089,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="21.75" thickBot="1">
+    <row r="48" spans="1:4" ht="15.75" thickBot="1">
       <c r="A48" s="9" t="s">
         <v>196</v>
       </c>
@@ -6030,15 +6097,15 @@
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A49" s="9" t="s">
+    <row r="49" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C49" s="9" t="s">
         <v>197</v>
       </c>
-      <c r="B49" s="10" t="s">
+      <c r="D49" s="10" t="s">
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="21.75" thickBot="1">
+    <row r="50" spans="1:4" ht="15.75" thickBot="1">
       <c r="A50" s="9" t="s">
         <v>199</v>
       </c>
@@ -6046,7 +6113,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="21.75" thickBot="1">
+    <row r="51" spans="1:4" ht="15.75" thickBot="1">
       <c r="A51" s="9" t="s">
         <v>201</v>
       </c>
@@ -6054,7 +6121,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="21.75" thickBot="1">
+    <row r="52" spans="1:4" ht="15.75" thickBot="1">
       <c r="A52" s="9" t="s">
         <v>203</v>
       </c>
@@ -6062,7 +6129,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="21.75" thickBot="1">
+    <row r="53" spans="1:4" ht="15.75" thickBot="1">
       <c r="A53" s="9" t="s">
         <v>205</v>
       </c>
@@ -6070,7 +6137,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15.75" thickBot="1">
+    <row r="54" spans="1:4" ht="15.75" thickBot="1">
       <c r="A54" s="9" t="s">
         <v>207</v>
       </c>
@@ -6078,7 +6145,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="15.75" thickBot="1">
+    <row r="55" spans="1:4" ht="15.75" thickBot="1">
       <c r="A55" s="9" t="s">
         <v>209</v>
       </c>
@@ -6086,7 +6153,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15.75" thickBot="1">
+    <row r="56" spans="1:4" ht="15.75" thickBot="1">
       <c r="A56" s="9" t="s">
         <v>211</v>
       </c>
@@ -6094,7 +6161,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="15.75" thickBot="1">
+    <row r="57" spans="1:4" ht="15.75" thickBot="1">
       <c r="A57" s="9" t="s">
         <v>213</v>
       </c>
@@ -6102,7 +6169,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15.75" thickBot="1">
+    <row r="58" spans="1:4" ht="15.75" thickBot="1">
       <c r="A58" s="9" t="s">
         <v>215</v>
       </c>
@@ -6110,7 +6177,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="15.75" thickBot="1">
+    <row r="59" spans="1:4" ht="15.75" thickBot="1">
       <c r="A59" s="9" t="s">
         <v>217</v>
       </c>
@@ -6118,7 +6185,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15.75" thickBot="1">
+    <row r="60" spans="1:4" ht="15.75" thickBot="1">
       <c r="A60" s="9" t="s">
         <v>219</v>
       </c>
@@ -6126,7 +6193,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="15.75" thickBot="1">
+    <row r="61" spans="1:4" ht="15.75" thickBot="1">
       <c r="A61" s="9" t="s">
         <v>221</v>
       </c>
@@ -6134,7 +6201,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="15.75" thickBot="1">
+    <row r="62" spans="1:4" ht="15.75" thickBot="1">
       <c r="A62" s="9" t="s">
         <v>223</v>
       </c>
@@ -6142,7 +6209,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15.75" thickBot="1">
+    <row r="63" spans="1:4" ht="15.75" thickBot="1">
       <c r="A63" s="9" t="s">
         <v>225</v>
       </c>
@@ -6150,7 +6217,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15.75" thickBot="1">
+    <row r="64" spans="1:4" ht="15.75" thickBot="1">
       <c r="A64" s="9" t="s">
         <v>227</v>
       </c>
@@ -6158,7 +6225,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="15.75" thickBot="1">
+    <row r="65" spans="1:4" ht="15.75" thickBot="1">
       <c r="A65" s="9" t="s">
         <v>229</v>
       </c>
@@ -6166,7 +6233,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="15.75" thickBot="1">
+    <row r="66" spans="1:4" ht="15.75" thickBot="1">
       <c r="A66" s="9" t="s">
         <v>231</v>
       </c>
@@ -6174,7 +6241,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="15.75" thickBot="1">
+    <row r="67" spans="1:4" ht="15.75" thickBot="1">
       <c r="A67" s="9" t="s">
         <v>233</v>
       </c>
@@ -6182,7 +6249,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="15.75" thickBot="1">
+    <row r="68" spans="1:4" ht="15.75" thickBot="1">
       <c r="A68" s="9" t="s">
         <v>235</v>
       </c>
@@ -6190,7 +6257,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="15.75" thickBot="1">
+    <row r="69" spans="1:4" ht="15.75" thickBot="1">
       <c r="A69" s="9" t="s">
         <v>236</v>
       </c>
@@ -6198,7 +6265,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:2" ht="15.75" thickBot="1">
+    <row r="70" spans="1:4" ht="15.75" thickBot="1">
       <c r="A70" s="9" t="s">
         <v>237</v>
       </c>
@@ -6206,15 +6273,15 @@
         <v>238</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A71" s="9" t="s">
+    <row r="71" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C71" s="9" t="s">
         <v>239</v>
       </c>
-      <c r="B71" s="10" t="s">
+      <c r="D71" s="10" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="15.75" thickBot="1">
+    <row r="72" spans="1:4" ht="15.75" thickBot="1">
       <c r="A72" s="7" t="s">
         <v>241</v>
       </c>
@@ -6222,7 +6289,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="73" spans="1:2" ht="15.75" thickBot="1">
+    <row r="73" spans="1:4" ht="15.75" thickBot="1">
       <c r="A73" s="9" t="s">
         <v>243</v>
       </c>
@@ -6230,7 +6297,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="74" spans="1:2" ht="15.75" thickBot="1">
+    <row r="74" spans="1:4" ht="15.75" thickBot="1">
       <c r="A74" s="9" t="s">
         <v>245</v>
       </c>
@@ -6238,7 +6305,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="75" spans="1:2" ht="15.75" thickBot="1">
+    <row r="75" spans="1:4" ht="15.75" thickBot="1">
       <c r="A75" s="9" t="s">
         <v>247</v>
       </c>
@@ -6246,7 +6313,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="76" spans="1:2" ht="15.75" thickBot="1">
+    <row r="76" spans="1:4" ht="15.75" thickBot="1">
       <c r="A76" s="9" t="s">
         <v>249</v>
       </c>
@@ -6254,7 +6321,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="77" spans="1:2" ht="15.75" thickBot="1">
+    <row r="77" spans="1:4" ht="15.75" thickBot="1">
       <c r="A77" s="9" t="s">
         <v>251</v>
       </c>
@@ -6262,7 +6329,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="78" spans="1:2" ht="15.75" thickBot="1">
+    <row r="78" spans="1:4" ht="15.75" thickBot="1">
       <c r="A78" s="9" t="s">
         <v>253</v>
       </c>
@@ -6270,7 +6337,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="79" spans="1:2" ht="15.75" thickBot="1">
+    <row r="79" spans="1:4" ht="15.75" thickBot="1">
       <c r="A79" s="9" t="s">
         <v>255</v>
       </c>
@@ -6278,39 +6345,39 @@
         <v>256</v>
       </c>
     </row>
-    <row r="80" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A80" s="7" t="s">
+    <row r="80" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C80" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="B80" s="8" t="s">
+      <c r="D80" s="8" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="81" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A81" s="9" t="s">
+    <row r="81" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C81" s="9" t="s">
         <v>258</v>
       </c>
-      <c r="B81" s="10" t="s">
+      <c r="D81" s="10" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="82" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A82" s="9" t="s">
+    <row r="82" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C82" s="9" t="s">
         <v>260</v>
       </c>
-      <c r="B82" s="10" t="s">
+      <c r="D82" s="10" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="83" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A83" s="9" t="s">
+    <row r="83" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C83" s="9" t="s">
         <v>262</v>
       </c>
-      <c r="B83" s="10" t="s">
+      <c r="D83" s="10" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="84" spans="1:2" ht="15.75" thickBot="1">
+    <row r="84" spans="1:4" ht="15.75" thickBot="1">
       <c r="A84" s="9" t="s">
         <v>264</v>
       </c>
@@ -6318,7 +6385,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="85" spans="1:2" ht="15.75" thickBot="1">
+    <row r="85" spans="1:4" ht="15.75" thickBot="1">
       <c r="A85" s="9" t="s">
         <v>266</v>
       </c>
@@ -6326,7 +6393,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="86" spans="1:2" ht="15.75" thickBot="1">
+    <row r="86" spans="1:4" ht="15.75" thickBot="1">
       <c r="A86" s="9" t="s">
         <v>268</v>
       </c>
@@ -6334,7 +6401,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="87" spans="1:2" ht="15.75" thickBot="1">
+    <row r="87" spans="1:4" ht="15.75" thickBot="1">
       <c r="A87" s="9" t="s">
         <v>270</v>
       </c>
@@ -6342,7 +6409,7 @@
         <v>271</v>
       </c>
     </row>
-    <row r="88" spans="1:2" ht="15.75" thickBot="1">
+    <row r="88" spans="1:4" ht="15.75" thickBot="1">
       <c r="A88" s="9" t="s">
         <v>272</v>
       </c>
@@ -6350,7 +6417,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="89" spans="1:2" ht="15.75" thickBot="1">
+    <row r="89" spans="1:4" ht="15.75" thickBot="1">
       <c r="A89" s="9" t="s">
         <v>274</v>
       </c>
@@ -6358,7 +6425,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="90" spans="1:2" ht="15.75" thickBot="1">
+    <row r="90" spans="1:4" ht="15.75" thickBot="1">
       <c r="A90" s="9" t="s">
         <v>276</v>
       </c>
@@ -6366,7 +6433,7 @@
         <v>277</v>
       </c>
     </row>
-    <row r="91" spans="1:2" ht="15.75" thickBot="1">
+    <row r="91" spans="1:4" ht="15.75" thickBot="1">
       <c r="A91" s="9" t="s">
         <v>71</v>
       </c>
@@ -6374,7 +6441,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="92" spans="1:2" ht="15.75" thickBot="1">
+    <row r="92" spans="1:4" ht="15.75" thickBot="1">
       <c r="A92" s="9" t="s">
         <v>279</v>
       </c>
@@ -6382,7 +6449,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="93" spans="1:2" ht="15.75" thickBot="1">
+    <row r="93" spans="1:4" ht="15.75" thickBot="1">
       <c r="A93" s="9" t="s">
         <v>119</v>
       </c>
@@ -6390,7 +6457,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="94" spans="1:2" ht="15.75" thickBot="1">
+    <row r="94" spans="1:4" ht="15.75" thickBot="1">
       <c r="A94" s="9" t="s">
         <v>282</v>
       </c>
@@ -6398,7 +6465,7 @@
         <v>283</v>
       </c>
     </row>
-    <row r="95" spans="1:2" ht="15.75" thickBot="1">
+    <row r="95" spans="1:4" ht="15.75" thickBot="1">
       <c r="A95" s="9" t="s">
         <v>284</v>
       </c>
@@ -6406,7 +6473,7 @@
         <v>285</v>
       </c>
     </row>
-    <row r="96" spans="1:2" ht="15.75" thickBot="1">
+    <row r="96" spans="1:4" ht="15.75" thickBot="1">
       <c r="A96" s="9" t="s">
         <v>286</v>
       </c>
@@ -6542,7 +6609,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="113" spans="1:2" ht="15.75" thickBot="1">
+    <row r="113" spans="1:4" ht="15.75" thickBot="1">
       <c r="A113" s="9" t="s">
         <v>91</v>
       </c>
@@ -6550,7 +6617,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="114" spans="1:2" ht="15.75" thickBot="1">
+    <row r="114" spans="1:4" ht="15.75" thickBot="1">
       <c r="A114" s="9" t="s">
         <v>313</v>
       </c>
@@ -6558,7 +6625,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="115" spans="1:2" ht="15.75" thickBot="1">
+    <row r="115" spans="1:4" ht="15.75" thickBot="1">
       <c r="A115" s="9" t="s">
         <v>315</v>
       </c>
@@ -6566,7 +6633,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="116" spans="1:2" ht="15.75" thickBot="1">
+    <row r="116" spans="1:4" ht="15.75" thickBot="1">
       <c r="A116" s="9" t="s">
         <v>317</v>
       </c>
@@ -6574,15 +6641,15 @@
         <v>318</v>
       </c>
     </row>
-    <row r="117" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A117" s="9" t="s">
+    <row r="117" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C117" s="9" t="s">
         <v>319</v>
       </c>
-      <c r="B117" s="10" t="s">
+      <c r="D117" s="10" t="s">
         <v>320</v>
       </c>
     </row>
-    <row r="118" spans="1:2" ht="15.75" thickBot="1">
+    <row r="118" spans="1:4" ht="15.75" thickBot="1">
       <c r="A118" s="9" t="s">
         <v>321</v>
       </c>
@@ -6590,7 +6657,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="119" spans="1:2" ht="15.75" thickBot="1">
+    <row r="119" spans="1:4" ht="15.75" thickBot="1">
       <c r="A119" s="7" t="s">
         <v>323</v>
       </c>
@@ -6598,7 +6665,7 @@
         <v>324</v>
       </c>
     </row>
-    <row r="120" spans="1:2" ht="15.75" thickBot="1">
+    <row r="120" spans="1:4" ht="15.75" thickBot="1">
       <c r="A120" s="9" t="s">
         <v>325</v>
       </c>
@@ -6606,7 +6673,7 @@
         <v>326</v>
       </c>
     </row>
-    <row r="121" spans="1:2" ht="15.75" thickBot="1">
+    <row r="121" spans="1:4" ht="15.75" thickBot="1">
       <c r="A121" s="9" t="s">
         <v>327</v>
       </c>
@@ -6614,7 +6681,7 @@
         <v>328</v>
       </c>
     </row>
-    <row r="122" spans="1:2" ht="15.75" thickBot="1">
+    <row r="122" spans="1:4" ht="15.75" thickBot="1">
       <c r="A122" s="9" t="s">
         <v>329</v>
       </c>
@@ -6622,7 +6689,7 @@
         <v>330</v>
       </c>
     </row>
-    <row r="123" spans="1:2" ht="15.75" thickBot="1">
+    <row r="123" spans="1:4" ht="15.75" thickBot="1">
       <c r="A123" s="9" t="s">
         <v>331</v>
       </c>
@@ -6630,7 +6697,7 @@
         <v>332</v>
       </c>
     </row>
-    <row r="124" spans="1:2" ht="15.75" thickBot="1">
+    <row r="124" spans="1:4" ht="15.75" thickBot="1">
       <c r="A124" s="9" t="s">
         <v>333</v>
       </c>
@@ -6638,7 +6705,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="125" spans="1:2" ht="15.75" thickBot="1">
+    <row r="125" spans="1:4" ht="15.75" thickBot="1">
       <c r="A125" s="9" t="s">
         <v>335</v>
       </c>
@@ -6646,7 +6713,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="126" spans="1:2" ht="15.75" thickBot="1">
+    <row r="126" spans="1:4" ht="15.75" thickBot="1">
       <c r="A126" s="9" t="s">
         <v>337</v>
       </c>
@@ -6654,7 +6721,7 @@
         <v>338</v>
       </c>
     </row>
-    <row r="127" spans="1:2" ht="15.75" thickBot="1">
+    <row r="127" spans="1:4" ht="15.75" thickBot="1">
       <c r="A127" s="9" t="s">
         <v>339</v>
       </c>
@@ -6662,7 +6729,7 @@
         <v>340</v>
       </c>
     </row>
-    <row r="128" spans="1:2" ht="15.75" thickBot="1">
+    <row r="128" spans="1:4" ht="15.75" thickBot="1">
       <c r="A128" s="9" t="s">
         <v>341</v>
       </c>
@@ -6670,7 +6737,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="129" spans="1:2" ht="21.75" thickBot="1">
+    <row r="129" spans="1:4" ht="21.75" thickBot="1">
       <c r="A129" s="9" t="s">
         <v>343</v>
       </c>
@@ -6678,7 +6745,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="130" spans="1:2" ht="15.75" thickBot="1">
+    <row r="130" spans="1:4" ht="15.75" thickBot="1">
       <c r="A130" s="9" t="s">
         <v>345</v>
       </c>
@@ -6686,7 +6753,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="131" spans="1:2" ht="15.75" thickBot="1">
+    <row r="131" spans="1:4" ht="15.75" thickBot="1">
       <c r="A131" s="9" t="s">
         <v>347</v>
       </c>
@@ -6694,7 +6761,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="132" spans="1:2" ht="15.75" thickBot="1">
+    <row r="132" spans="1:4" ht="15.75" thickBot="1">
       <c r="A132" s="9" t="s">
         <v>349</v>
       </c>
@@ -6702,7 +6769,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="133" spans="1:2" ht="15.75" thickBot="1">
+    <row r="133" spans="1:4" ht="15.75" thickBot="1">
       <c r="A133" s="9" t="s">
         <v>351</v>
       </c>
@@ -6710,7 +6777,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="134" spans="1:2" ht="15.75" thickBot="1">
+    <row r="134" spans="1:4" ht="15.75" thickBot="1">
       <c r="A134" s="9" t="s">
         <v>353</v>
       </c>
@@ -6718,7 +6785,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="135" spans="1:2" ht="15.75" thickBot="1">
+    <row r="135" spans="1:4" ht="15.75" thickBot="1">
       <c r="A135" s="9" t="s">
         <v>355</v>
       </c>
@@ -6726,7 +6793,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="136" spans="1:2" ht="15.75" thickBot="1">
+    <row r="136" spans="1:4" ht="15.75" thickBot="1">
       <c r="A136" s="9" t="s">
         <v>357</v>
       </c>
@@ -6734,7 +6801,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="137" spans="1:2" ht="15.75" thickBot="1">
+    <row r="137" spans="1:4" ht="15.75" thickBot="1">
       <c r="A137" s="9" t="s">
         <v>359</v>
       </c>
@@ -6742,7 +6809,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="138" spans="1:2" ht="15.75" thickBot="1">
+    <row r="138" spans="1:4" ht="15.75" thickBot="1">
       <c r="A138" s="9" t="s">
         <v>361</v>
       </c>
@@ -6750,7 +6817,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="139" spans="1:2" ht="15.75" thickBot="1">
+    <row r="139" spans="1:4" ht="15.75" thickBot="1">
       <c r="A139" s="9" t="s">
         <v>363</v>
       </c>
@@ -6758,7 +6825,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="140" spans="1:2" ht="15.75" thickBot="1">
+    <row r="140" spans="1:4" ht="15.75" thickBot="1">
       <c r="A140" s="9" t="s">
         <v>365</v>
       </c>
@@ -6766,7 +6833,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="141" spans="1:2" ht="15.75" thickBot="1">
+    <row r="141" spans="1:4" ht="15.75" thickBot="1">
       <c r="A141" s="9" t="s">
         <v>367</v>
       </c>
@@ -6774,7 +6841,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="142" spans="1:2" ht="15.75" thickBot="1">
+    <row r="142" spans="1:4" ht="15.75" thickBot="1">
       <c r="A142" s="9" t="s">
         <v>369</v>
       </c>
@@ -6782,7 +6849,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="143" spans="1:2" ht="15.75" thickBot="1">
+    <row r="143" spans="1:4" ht="15.75" thickBot="1">
       <c r="A143" s="9" t="s">
         <v>371</v>
       </c>
@@ -6790,31 +6857,31 @@
         <v>372</v>
       </c>
     </row>
-    <row r="144" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A144" s="9" t="s">
+    <row r="144" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C144" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B144" s="10" t="s">
+      <c r="D144" s="10" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="145" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A145" s="9" t="s">
+    <row r="145" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C145" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="B145" s="10" t="s">
+      <c r="D145" s="10" t="s">
         <v>374</v>
       </c>
     </row>
-    <row r="146" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A146" s="9" t="s">
+    <row r="146" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C146" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="B146" s="10" t="s">
+      <c r="D146" s="10" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="147" spans="1:2" ht="15.75" thickBot="1">
+    <row r="147" spans="1:4" ht="15.75" thickBot="1">
       <c r="A147" s="9" t="s">
         <v>376</v>
       </c>
@@ -6822,7 +6889,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="148" spans="1:2" ht="15.75" thickBot="1">
+    <row r="148" spans="1:4" ht="15.75" thickBot="1">
       <c r="A148" s="9" t="s">
         <v>378</v>
       </c>
@@ -6830,7 +6897,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="149" spans="1:2" ht="15.75" thickBot="1">
+    <row r="149" spans="1:4" ht="15.75" thickBot="1">
       <c r="A149" s="9" t="s">
         <v>380</v>
       </c>
@@ -6838,7 +6905,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="150" spans="1:2" ht="15.75" thickBot="1">
+    <row r="150" spans="1:4" ht="15.75" thickBot="1">
       <c r="A150" s="9" t="s">
         <v>382</v>
       </c>
@@ -6846,7 +6913,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="151" spans="1:2" ht="15.75" thickBot="1">
+    <row r="151" spans="1:4" ht="15.75" thickBot="1">
       <c r="A151" s="9" t="s">
         <v>384</v>
       </c>
@@ -6854,7 +6921,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="152" spans="1:2" ht="15.75" thickBot="1">
+    <row r="152" spans="1:4" ht="15.75" thickBot="1">
       <c r="A152" s="9" t="s">
         <v>386</v>
       </c>
@@ -6862,7 +6929,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="153" spans="1:2" ht="15.75" thickBot="1">
+    <row r="153" spans="1:4" ht="15.75" thickBot="1">
       <c r="A153" s="9" t="s">
         <v>388</v>
       </c>
@@ -6870,7 +6937,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="154" spans="1:2" ht="15.75" thickBot="1">
+    <row r="154" spans="1:4" ht="15.75" thickBot="1">
       <c r="A154" s="9" t="s">
         <v>390</v>
       </c>
@@ -6878,7 +6945,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="155" spans="1:2" ht="15.75" thickBot="1">
+    <row r="155" spans="1:4" ht="15.75" thickBot="1">
       <c r="A155" s="9" t="s">
         <v>392</v>
       </c>
@@ -6886,7 +6953,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="156" spans="1:2" ht="15.75" thickBot="1">
+    <row r="156" spans="1:4" ht="15.75" thickBot="1">
       <c r="A156" s="9" t="s">
         <v>394</v>
       </c>
@@ -6894,7 +6961,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="157" spans="1:2" ht="15.75" thickBot="1">
+    <row r="157" spans="1:4" ht="15.75" thickBot="1">
       <c r="A157" s="7" t="s">
         <v>396</v>
       </c>
@@ -6902,7 +6969,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="158" spans="1:2" ht="15.75" thickBot="1">
+    <row r="158" spans="1:4" ht="15.75" thickBot="1">
       <c r="A158" s="9" t="s">
         <v>398</v>
       </c>
@@ -6910,7 +6977,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="159" spans="1:2" ht="15.75" thickBot="1">
+    <row r="159" spans="1:4" ht="15.75" thickBot="1">
       <c r="A159" s="9" t="s">
         <v>400</v>
       </c>
@@ -6918,11 +6985,11 @@
         <v>401</v>
       </c>
     </row>
-    <row r="160" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A160" s="9" t="s">
+    <row r="160" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C160" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B160" s="10" t="s">
+      <c r="D160" s="10" t="s">
         <v>402</v>
       </c>
     </row>
@@ -7054,7 +7121,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="177" spans="1:2" ht="15.75" thickBot="1">
+    <row r="177" spans="1:4" ht="15.75" thickBot="1">
       <c r="A177" s="9" t="s">
         <v>431</v>
       </c>
@@ -7062,7 +7129,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="178" spans="1:2" ht="15.75" thickBot="1">
+    <row r="178" spans="1:4" ht="15.75" thickBot="1">
       <c r="A178" s="9" t="s">
         <v>433</v>
       </c>
@@ -7070,7 +7137,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="179" spans="1:2" ht="15.75" thickBot="1">
+    <row r="179" spans="1:4" ht="15.75" thickBot="1">
       <c r="A179" s="9" t="s">
         <v>435</v>
       </c>
@@ -7078,7 +7145,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="180" spans="1:2" ht="15.75" thickBot="1">
+    <row r="180" spans="1:4" ht="15.75" thickBot="1">
       <c r="A180" s="9" t="s">
         <v>437</v>
       </c>
@@ -7086,15 +7153,15 @@
         <v>438</v>
       </c>
     </row>
-    <row r="181" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A181" s="9" t="s">
+    <row r="181" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C181" s="9" t="s">
         <v>439</v>
       </c>
-      <c r="B181" s="10" t="s">
+      <c r="D181" s="10" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="182" spans="1:2" ht="15.75" thickBot="1">
+    <row r="182" spans="1:4" ht="15.75" thickBot="1">
       <c r="A182" s="9" t="s">
         <v>441</v>
       </c>
@@ -7102,15 +7169,15 @@
         <v>442</v>
       </c>
     </row>
-    <row r="183" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A183" s="9" t="s">
+    <row r="183" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C183" s="9" t="s">
         <v>92</v>
       </c>
-      <c r="B183" s="10" t="s">
+      <c r="D183" s="10" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="184" spans="1:2" ht="15.75" thickBot="1">
+    <row r="184" spans="1:4" ht="15.75" thickBot="1">
       <c r="A184" s="9" t="s">
         <v>444</v>
       </c>
@@ -7118,7 +7185,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="185" spans="1:2" ht="15.75" thickBot="1">
+    <row r="185" spans="1:4" ht="15.75" thickBot="1">
       <c r="A185" s="9" t="s">
         <v>446</v>
       </c>
@@ -7126,7 +7193,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="186" spans="1:2" ht="15.75" thickBot="1">
+    <row r="186" spans="1:4" ht="15.75" thickBot="1">
       <c r="A186" s="9" t="s">
         <v>448</v>
       </c>
@@ -7134,7 +7201,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="187" spans="1:2" ht="15.75" thickBot="1">
+    <row r="187" spans="1:4" ht="15.75" thickBot="1">
       <c r="A187" s="9" t="s">
         <v>114</v>
       </c>
@@ -7142,7 +7209,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="188" spans="1:2" ht="15.75" thickBot="1">
+    <row r="188" spans="1:4" ht="15.75" thickBot="1">
       <c r="A188" s="9" t="s">
         <v>451</v>
       </c>
@@ -7150,7 +7217,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="189" spans="1:2" ht="15.75" thickBot="1">
+    <row r="189" spans="1:4" ht="15.75" thickBot="1">
       <c r="A189" s="9" t="s">
         <v>90</v>
       </c>
@@ -7158,39 +7225,39 @@
         <v>453</v>
       </c>
     </row>
-    <row r="190" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A190" s="9" t="s">
+    <row r="190" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C190" s="9" t="s">
         <v>454</v>
       </c>
-      <c r="B190" s="10" t="s">
+      <c r="D190" s="10" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="191" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A191" s="9" t="s">
+    <row r="191" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C191" s="9" t="s">
         <v>456</v>
       </c>
-      <c r="B191" s="10" t="s">
+      <c r="D191" s="10" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="192" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A192" s="9" t="s">
+    <row r="192" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C192" s="9" t="s">
         <v>458</v>
       </c>
-      <c r="B192" s="10" t="s">
+      <c r="D192" s="10" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="193" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A193" s="9" t="s">
+    <row r="193" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C193" s="9" t="s">
         <v>460</v>
       </c>
-      <c r="B193" s="10" t="s">
+      <c r="D193" s="10" t="s">
         <v>461</v>
       </c>
     </row>
-    <row r="194" spans="1:2" ht="15.75" thickBot="1">
+    <row r="194" spans="1:4" ht="15.75" thickBot="1">
       <c r="A194" s="9" t="s">
         <v>462</v>
       </c>
@@ -7198,7 +7265,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="195" spans="1:2" ht="15.75" thickBot="1">
+    <row r="195" spans="1:4" ht="15.75" thickBot="1">
       <c r="A195" s="9" t="s">
         <v>464</v>
       </c>
@@ -7206,7 +7273,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="196" spans="1:2" ht="15.75" thickBot="1">
+    <row r="196" spans="1:4" ht="15.75" thickBot="1">
       <c r="A196" s="7" t="s">
         <v>466</v>
       </c>
@@ -7214,7 +7281,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="197" spans="1:2" ht="15.75" thickBot="1">
+    <row r="197" spans="1:4" ht="15.75" thickBot="1">
       <c r="A197" s="9" t="s">
         <v>468</v>
       </c>
@@ -7222,7 +7289,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="198" spans="1:2" ht="15.75" thickBot="1">
+    <row r="198" spans="1:4" ht="15.75" thickBot="1">
       <c r="A198" s="9" t="s">
         <v>470</v>
       </c>
@@ -7230,7 +7297,7 @@
         <v>471</v>
       </c>
     </row>
-    <row r="199" spans="1:2" ht="21.75" thickBot="1">
+    <row r="199" spans="1:4" ht="21.75" thickBot="1">
       <c r="A199" s="9" t="s">
         <v>472</v>
       </c>
@@ -7238,319 +7305,319 @@
         <v>473</v>
       </c>
     </row>
-    <row r="200" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A200" s="9" t="s">
+    <row r="200" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C200" s="9" t="s">
         <v>474</v>
       </c>
-      <c r="B200" s="10" t="s">
+      <c r="D200" s="10" t="s">
         <v>475</v>
       </c>
     </row>
-    <row r="201" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A201" s="9" t="s">
+    <row r="201" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C201" s="9" t="s">
         <v>476</v>
       </c>
-      <c r="B201" s="10" t="s">
+      <c r="D201" s="10" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="202" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A202" s="9" t="s">
+    <row r="202" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C202" s="9" t="s">
         <v>478</v>
       </c>
-      <c r="B202" s="10" t="s">
+      <c r="D202" s="10" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="203" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A203" s="9" t="s">
+    <row r="203" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C203" s="9" t="s">
         <v>480</v>
       </c>
-      <c r="B203" s="10" t="s">
+      <c r="D203" s="10" t="s">
         <v>481</v>
       </c>
     </row>
-    <row r="204" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A204" s="9" t="s">
+    <row r="204" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C204" s="9" t="s">
         <v>482</v>
       </c>
-      <c r="B204" s="10" t="s">
+      <c r="D204" s="10" t="s">
         <v>483</v>
       </c>
     </row>
-    <row r="205" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A205" s="9" t="s">
+    <row r="205" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C205" s="9" t="s">
         <v>484</v>
       </c>
-      <c r="B205" s="10" t="s">
+      <c r="D205" s="10" t="s">
         <v>485</v>
       </c>
     </row>
-    <row r="206" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A206" s="9" t="s">
+    <row r="206" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C206" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="B206" s="10" t="s">
+      <c r="D206" s="10" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="207" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A207" s="9" t="s">
+    <row r="207" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C207" s="9" t="s">
         <v>488</v>
       </c>
-      <c r="B207" s="10" t="s">
+      <c r="D207" s="10" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="208" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A208" s="9" t="s">
+    <row r="208" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C208" s="9" t="s">
         <v>490</v>
       </c>
-      <c r="B208" s="10" t="s">
+      <c r="D208" s="10" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="209" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A209" s="9" t="s">
+    <row r="209" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C209" s="9" t="s">
         <v>492</v>
       </c>
-      <c r="B209" s="10" t="s">
+      <c r="D209" s="10" t="s">
         <v>493</v>
       </c>
     </row>
-    <row r="210" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A210" s="9" t="s">
+    <row r="210" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C210" s="9" t="s">
         <v>494</v>
       </c>
-      <c r="B210" s="10" t="s">
+      <c r="D210" s="10" t="s">
         <v>495</v>
       </c>
     </row>
-    <row r="211" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A211" s="9" t="s">
+    <row r="211" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C211" s="9" t="s">
         <v>496</v>
       </c>
-      <c r="B211" s="10" t="s">
+      <c r="D211" s="10" t="s">
         <v>497</v>
       </c>
     </row>
-    <row r="212" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A212" s="9" t="s">
+    <row r="212" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C212" s="9" t="s">
         <v>498</v>
       </c>
-      <c r="B212" s="10" t="s">
+      <c r="D212" s="10" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="213" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A213" s="9" t="s">
+    <row r="213" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C213" s="9" t="s">
         <v>500</v>
       </c>
-      <c r="B213" s="10" t="s">
+      <c r="D213" s="10" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="214" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A214" s="9" t="s">
+    <row r="214" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C214" s="9" t="s">
         <v>502</v>
       </c>
-      <c r="B214" s="10" t="s">
+      <c r="D214" s="10" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="215" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A215" s="9" t="s">
+    <row r="215" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C215" s="9" t="s">
         <v>504</v>
       </c>
-      <c r="B215" s="10" t="s">
+      <c r="D215" s="10" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="216" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A216" s="9" t="s">
+    <row r="216" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C216" s="9" t="s">
         <v>506</v>
       </c>
-      <c r="B216" s="10" t="s">
+      <c r="D216" s="10" t="s">
         <v>507</v>
       </c>
     </row>
-    <row r="217" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A217" s="9" t="s">
+    <row r="217" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C217" s="9" t="s">
         <v>508</v>
       </c>
-      <c r="B217" s="10" t="s">
+      <c r="D217" s="10" t="s">
         <v>509</v>
       </c>
     </row>
-    <row r="218" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A218" s="9" t="s">
+    <row r="218" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C218" s="9" t="s">
         <v>510</v>
       </c>
-      <c r="B218" s="10" t="s">
+      <c r="D218" s="10" t="s">
         <v>511</v>
       </c>
     </row>
-    <row r="219" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A219" s="9" t="s">
+    <row r="219" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C219" s="9" t="s">
         <v>512</v>
       </c>
-      <c r="B219" s="10" t="s">
+      <c r="D219" s="10" t="s">
         <v>513</v>
       </c>
     </row>
-    <row r="220" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A220" s="9" t="s">
+    <row r="220" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C220" s="9" t="s">
         <v>514</v>
       </c>
-      <c r="B220" s="10" t="s">
+      <c r="D220" s="10" t="s">
         <v>515</v>
       </c>
     </row>
-    <row r="221" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A221" s="9" t="s">
+    <row r="221" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C221" s="9" t="s">
         <v>516</v>
       </c>
-      <c r="B221" s="10" t="s">
+      <c r="D221" s="10" t="s">
         <v>517</v>
       </c>
     </row>
-    <row r="222" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A222" s="9" t="s">
+    <row r="222" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C222" s="9" t="s">
         <v>518</v>
       </c>
-      <c r="B222" s="10" t="s">
+      <c r="D222" s="10" t="s">
         <v>519</v>
       </c>
     </row>
-    <row r="223" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A223" s="9" t="s">
+    <row r="223" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C223" s="9" t="s">
         <v>520</v>
       </c>
-      <c r="B223" s="10" t="s">
+      <c r="D223" s="10" t="s">
         <v>521</v>
       </c>
     </row>
-    <row r="224" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A224" s="9" t="s">
+    <row r="224" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C224" s="9" t="s">
         <v>522</v>
       </c>
-      <c r="B224" s="10" t="s">
+      <c r="D224" s="10" t="s">
         <v>523</v>
       </c>
     </row>
-    <row r="225" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A225" s="9" t="s">
+    <row r="225" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C225" s="9" t="s">
         <v>524</v>
       </c>
-      <c r="B225" s="10" t="s">
+      <c r="D225" s="10" t="s">
         <v>525</v>
       </c>
     </row>
-    <row r="226" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A226" s="9" t="s">
+    <row r="226" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C226" s="9" t="s">
         <v>526</v>
       </c>
-      <c r="B226" s="10" t="s">
+      <c r="D226" s="10" t="s">
         <v>527</v>
       </c>
     </row>
-    <row r="227" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A227" s="9" t="s">
+    <row r="227" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C227" s="9" t="s">
         <v>528</v>
       </c>
-      <c r="B227" s="10" t="s">
+      <c r="D227" s="10" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="228" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A228" s="9" t="s">
+    <row r="228" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C228" s="9" t="s">
         <v>529</v>
       </c>
-      <c r="B228" s="10" t="s">
+      <c r="D228" s="10" t="s">
         <v>530</v>
       </c>
     </row>
-    <row r="229" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A229" s="9" t="s">
+    <row r="229" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C229" s="9" t="s">
         <v>531</v>
       </c>
-      <c r="B229" s="10" t="s">
+      <c r="D229" s="10" t="s">
         <v>532</v>
       </c>
     </row>
-    <row r="230" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A230" s="9" t="s">
+    <row r="230" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C230" s="9" t="s">
         <v>533</v>
       </c>
-      <c r="B230" s="10" t="s">
+      <c r="D230" s="10" t="s">
         <v>534</v>
       </c>
     </row>
-    <row r="231" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A231" s="9" t="s">
+    <row r="231" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C231" s="9" t="s">
         <v>535</v>
       </c>
-      <c r="B231" s="10" t="s">
+      <c r="D231" s="10" t="s">
         <v>536</v>
       </c>
     </row>
-    <row r="232" spans="1:2" ht="21.75" thickBot="1">
-      <c r="A232" s="9" t="s">
+    <row r="232" spans="1:4" ht="32.25" thickBot="1">
+      <c r="C232" s="9" t="s">
         <v>537</v>
       </c>
-      <c r="B232" s="10" t="s">
+      <c r="D232" s="10" t="s">
         <v>538</v>
       </c>
     </row>
-    <row r="233" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A233" s="9" t="s">
+    <row r="233" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C233" s="9" t="s">
         <v>539</v>
       </c>
-      <c r="B233" s="10" t="s">
+      <c r="D233" s="10" t="s">
         <v>540</v>
       </c>
     </row>
-    <row r="234" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A234" s="7" t="s">
+    <row r="234" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C234" s="7" t="s">
         <v>541</v>
       </c>
-      <c r="B234" s="8" t="s">
+      <c r="D234" s="8" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="235" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A235" s="9" t="s">
+    <row r="235" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C235" s="9" t="s">
         <v>543</v>
       </c>
-      <c r="B235" s="10" t="s">
+      <c r="D235" s="10" t="s">
         <v>544</v>
       </c>
     </row>
-    <row r="236" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A236" s="9" t="s">
+    <row r="236" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C236" s="9" t="s">
         <v>545</v>
       </c>
-      <c r="B236" s="10" t="s">
+      <c r="D236" s="10" t="s">
         <v>546</v>
       </c>
     </row>
-    <row r="237" spans="1:2" ht="21.75" thickBot="1">
-      <c r="A237" s="9" t="s">
+    <row r="237" spans="1:4" ht="32.25" thickBot="1">
+      <c r="C237" s="9" t="s">
         <v>547</v>
       </c>
-      <c r="B237" s="10" t="s">
+      <c r="D237" s="10" t="s">
         <v>548</v>
       </c>
     </row>
-    <row r="238" spans="1:2" ht="21.75" thickBot="1">
-      <c r="A238" s="9" t="s">
+    <row r="238" spans="1:4" ht="32.25" thickBot="1">
+      <c r="C238" s="9" t="s">
         <v>549</v>
       </c>
-      <c r="B238" s="10" t="s">
+      <c r="D238" s="10" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="239" spans="1:2" ht="15.75" thickBot="1">
+    <row r="239" spans="1:4" ht="15.75" thickBot="1">
       <c r="A239" s="9" t="s">
         <v>550</v>
       </c>
@@ -7558,23 +7625,23 @@
         <v>551</v>
       </c>
     </row>
-    <row r="240" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A240" s="9" t="s">
+    <row r="240" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C240" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B240" s="10" t="s">
+      <c r="D240" s="10" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="241" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A241" s="9" t="s">
+    <row r="241" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C241" s="9" t="s">
         <v>553</v>
       </c>
-      <c r="B241" s="10" t="s">
+      <c r="D241" s="10" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="242" spans="1:2" ht="15.75" thickBot="1">
+    <row r="242" spans="1:4" ht="15.75" thickBot="1">
       <c r="A242" s="9" t="s">
         <v>555</v>
       </c>
@@ -7582,7 +7649,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="243" spans="1:2" ht="15.75" thickBot="1">
+    <row r="243" spans="1:4" ht="15.75" thickBot="1">
       <c r="A243" s="9" t="s">
         <v>557</v>
       </c>
@@ -7590,7 +7657,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="244" spans="1:2" ht="15.75" thickBot="1">
+    <row r="244" spans="1:4" ht="15.75" thickBot="1">
       <c r="A244" s="9" t="s">
         <v>559</v>
       </c>
@@ -7598,7 +7665,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="245" spans="1:2" ht="15.75" thickBot="1">
+    <row r="245" spans="1:4" ht="15.75" thickBot="1">
       <c r="A245" s="9" t="s">
         <v>561</v>
       </c>
@@ -7606,7 +7673,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="246" spans="1:2" ht="21.75" thickBot="1">
+    <row r="246" spans="1:4" ht="21.75" thickBot="1">
       <c r="A246" s="9" t="s">
         <v>563</v>
       </c>
@@ -7614,7 +7681,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="247" spans="1:2" ht="15.75" thickBot="1">
+    <row r="247" spans="1:4" ht="15.75" thickBot="1">
       <c r="A247" s="9" t="s">
         <v>565</v>
       </c>
@@ -7622,7 +7689,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="248" spans="1:2" ht="15.75" thickBot="1">
+    <row r="248" spans="1:4" ht="15.75" thickBot="1">
       <c r="A248" s="9" t="s">
         <v>567</v>
       </c>
@@ -7630,7 +7697,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="249" spans="1:2" ht="15.75" thickBot="1">
+    <row r="249" spans="1:4" ht="15.75" thickBot="1">
       <c r="A249" s="9" t="s">
         <v>569</v>
       </c>
@@ -7638,7 +7705,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="250" spans="1:2" ht="15.75" thickBot="1">
+    <row r="250" spans="1:4" ht="15.75" thickBot="1">
       <c r="A250" s="9" t="s">
         <v>571</v>
       </c>
@@ -7646,7 +7713,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="251" spans="1:2" ht="15.75" thickBot="1">
+    <row r="251" spans="1:4" ht="15.75" thickBot="1">
       <c r="A251" s="9" t="s">
         <v>573</v>
       </c>
@@ -7654,7 +7721,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="252" spans="1:2" ht="15.75" thickBot="1">
+    <row r="252" spans="1:4" ht="15.75" thickBot="1">
       <c r="A252" s="9" t="s">
         <v>575</v>
       </c>
@@ -7662,7 +7729,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="253" spans="1:2" ht="15.75" thickBot="1">
+    <row r="253" spans="1:4" ht="15.75" thickBot="1">
       <c r="A253" s="9" t="s">
         <v>577</v>
       </c>
@@ -7670,7 +7737,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="254" spans="1:2" ht="21.75" thickBot="1">
+    <row r="254" spans="1:4" ht="21.75" thickBot="1">
       <c r="A254" s="9" t="s">
         <v>579</v>
       </c>
@@ -7678,7 +7745,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="255" spans="1:2" ht="15.75" thickBot="1">
+    <row r="255" spans="1:4" ht="15.75" thickBot="1">
       <c r="A255" s="9" t="s">
         <v>581</v>
       </c>
@@ -7686,7 +7753,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="256" spans="1:2" ht="15.75" thickBot="1">
+    <row r="256" spans="1:4" ht="15.75" thickBot="1">
       <c r="A256" s="9" t="s">
         <v>583</v>
       </c>
@@ -7694,7 +7761,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="257" spans="1:2" ht="15.75" thickBot="1">
+    <row r="257" spans="1:4" ht="15.75" thickBot="1">
       <c r="A257" s="9" t="s">
         <v>585</v>
       </c>
@@ -7702,7 +7769,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="258" spans="1:2" ht="15.75" thickBot="1">
+    <row r="258" spans="1:4" ht="15.75" thickBot="1">
       <c r="A258" s="9" t="s">
         <v>587</v>
       </c>
@@ -7710,7 +7777,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="259" spans="1:2" ht="15.75" thickBot="1">
+    <row r="259" spans="1:4" ht="15.75" thickBot="1">
       <c r="A259" s="9" t="s">
         <v>589</v>
       </c>
@@ -7718,15 +7785,15 @@
         <v>590</v>
       </c>
     </row>
-    <row r="260" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A260" s="9" t="s">
+    <row r="260" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C260" s="9" t="s">
         <v>591</v>
       </c>
-      <c r="B260" s="10" t="s">
+      <c r="D260" s="10" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="261" spans="1:2" ht="15.75" thickBot="1">
+    <row r="261" spans="1:4" ht="15.75" thickBot="1">
       <c r="A261" s="9" t="s">
         <v>593</v>
       </c>
@@ -7734,7 +7801,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="262" spans="1:2" ht="15.75" thickBot="1">
+    <row r="262" spans="1:4" ht="15.75" thickBot="1">
       <c r="A262" s="9" t="s">
         <v>595</v>
       </c>
@@ -7742,7 +7809,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="263" spans="1:2" ht="15.75" thickBot="1">
+    <row r="263" spans="1:4" ht="15.75" thickBot="1">
       <c r="A263" s="9" t="s">
         <v>597</v>
       </c>
@@ -7750,7 +7817,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="264" spans="1:2" ht="21.75" thickBot="1">
+    <row r="264" spans="1:4" ht="21.75" thickBot="1">
       <c r="A264" s="9" t="s">
         <v>599</v>
       </c>
@@ -7758,7 +7825,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="265" spans="1:2" ht="15.75" thickBot="1">
+    <row r="265" spans="1:4" ht="15.75" thickBot="1">
       <c r="A265" s="9" t="s">
         <v>113</v>
       </c>
@@ -7766,7 +7833,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="266" spans="1:2" ht="15.75" thickBot="1">
+    <row r="266" spans="1:4" ht="15.75" thickBot="1">
       <c r="A266" s="9" t="s">
         <v>602</v>
       </c>
@@ -7774,7 +7841,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="267" spans="1:2" ht="15.75" thickBot="1">
+    <row r="267" spans="1:4" ht="15.75" thickBot="1">
       <c r="A267" s="9" t="s">
         <v>604</v>
       </c>
@@ -7782,7 +7849,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="268" spans="1:2" ht="15.75" thickBot="1">
+    <row r="268" spans="1:4" ht="15.75" thickBot="1">
       <c r="A268" s="9" t="s">
         <v>606</v>
       </c>
@@ -7790,7 +7857,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="269" spans="1:2" ht="15.75" thickBot="1">
+    <row r="269" spans="1:4" ht="15.75" thickBot="1">
       <c r="A269" s="7" t="s">
         <v>608</v>
       </c>
@@ -7798,7 +7865,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="270" spans="1:2" ht="15.75" thickBot="1">
+    <row r="270" spans="1:4" ht="15.75" thickBot="1">
       <c r="A270" s="9" t="s">
         <v>610</v>
       </c>
@@ -7806,7 +7873,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="271" spans="1:2" ht="15.75" thickBot="1">
+    <row r="271" spans="1:4" ht="15.75" thickBot="1">
       <c r="A271" s="9" t="s">
         <v>612</v>
       </c>
@@ -7814,7 +7881,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="272" spans="1:2" ht="15.75" thickBot="1">
+    <row r="272" spans="1:4" ht="15.75" thickBot="1">
       <c r="A272" s="9" t="s">
         <v>614</v>
       </c>
@@ -7822,7 +7889,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="273" spans="1:2" ht="15.75" thickBot="1">
+    <row r="273" spans="1:4" ht="15.75" thickBot="1">
       <c r="A273" s="9" t="s">
         <v>615</v>
       </c>
@@ -7830,7 +7897,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="274" spans="1:2" ht="15.75" thickBot="1">
+    <row r="274" spans="1:4" ht="15.75" thickBot="1">
       <c r="A274" s="9" t="s">
         <v>617</v>
       </c>
@@ -7838,7 +7905,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="275" spans="1:2" ht="15.75" thickBot="1">
+    <row r="275" spans="1:4" ht="15.75" thickBot="1">
       <c r="A275" s="9" t="s">
         <v>619</v>
       </c>
@@ -7846,7 +7913,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="276" spans="1:2" ht="15.75" thickBot="1">
+    <row r="276" spans="1:4" ht="15.75" thickBot="1">
       <c r="A276" s="9" t="s">
         <v>621</v>
       </c>
@@ -7854,7 +7921,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="277" spans="1:2" ht="15.75" thickBot="1">
+    <row r="277" spans="1:4" ht="15.75" thickBot="1">
       <c r="A277" s="9" t="s">
         <v>623</v>
       </c>
@@ -7862,7 +7929,7 @@
         <v>624</v>
       </c>
     </row>
-    <row r="278" spans="1:2" ht="15.75" thickBot="1">
+    <row r="278" spans="1:4" ht="15.75" thickBot="1">
       <c r="A278" s="9" t="s">
         <v>625</v>
       </c>
@@ -7870,7 +7937,7 @@
         <v>626</v>
       </c>
     </row>
-    <row r="279" spans="1:2" ht="15.75" thickBot="1">
+    <row r="279" spans="1:4" ht="15.75" thickBot="1">
       <c r="A279" s="9" t="s">
         <v>627</v>
       </c>
@@ -7878,7 +7945,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="280" spans="1:2" ht="15.75" thickBot="1">
+    <row r="280" spans="1:4" ht="15.75" thickBot="1">
       <c r="A280" s="9" t="s">
         <v>629</v>
       </c>
@@ -7886,15 +7953,15 @@
         <v>630</v>
       </c>
     </row>
-    <row r="281" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A281" s="9" t="s">
+    <row r="281" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C281" s="9" t="s">
         <v>631</v>
       </c>
-      <c r="B281" s="10" t="s">
+      <c r="D281" s="10" t="s">
         <v>632</v>
       </c>
     </row>
-    <row r="282" spans="1:2" ht="15.75" thickBot="1">
+    <row r="282" spans="1:4" ht="15.75" thickBot="1">
       <c r="A282" s="9" t="s">
         <v>633</v>
       </c>
@@ -7902,7 +7969,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="283" spans="1:2" ht="15.75" thickBot="1">
+    <row r="283" spans="1:4" ht="15.75" thickBot="1">
       <c r="A283" s="9" t="s">
         <v>118</v>
       </c>
@@ -7910,7 +7977,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="284" spans="1:2" ht="15.75" thickBot="1">
+    <row r="284" spans="1:4" ht="15.75" thickBot="1">
       <c r="A284" s="9" t="s">
         <v>98</v>
       </c>
@@ -7918,7 +7985,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="285" spans="1:2" ht="15.75" thickBot="1">
+    <row r="285" spans="1:4" ht="15.75" thickBot="1">
       <c r="A285" s="9" t="s">
         <v>81</v>
       </c>
@@ -7926,7 +7993,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="286" spans="1:2" ht="15.75" thickBot="1">
+    <row r="286" spans="1:4" ht="15.75" thickBot="1">
       <c r="A286" s="9" t="s">
         <v>62</v>
       </c>
@@ -7934,7 +8001,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="287" spans="1:2" ht="15.75" thickBot="1">
+    <row r="287" spans="1:4" ht="15.75" thickBot="1">
       <c r="A287" s="9" t="s">
         <v>80</v>
       </c>
@@ -7942,7 +8009,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="288" spans="1:2" ht="15.75" thickBot="1">
+    <row r="288" spans="1:4" ht="15.75" thickBot="1">
       <c r="A288" s="9" t="s">
         <v>636</v>
       </c>
@@ -11069,14 +11136,920 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="B2:Y37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16" style="23" customWidth="1"/>
+    <col min="2" max="2" width="19" style="23" customWidth="1"/>
+    <col min="3" max="4" width="9.140625" style="23"/>
+    <col min="5" max="5" width="13.5703125" style="23" customWidth="1"/>
+    <col min="6" max="7" width="9.140625" style="23"/>
+    <col min="8" max="8" width="21.28515625" style="23" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="23"/>
+    <col min="10" max="10" width="14.5703125" style="23" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" style="23" customWidth="1"/>
+    <col min="12" max="14" width="9.140625" style="23"/>
+    <col min="15" max="15" width="12.5703125" style="23" customWidth="1"/>
+    <col min="16" max="17" width="9.140625" style="23"/>
+    <col min="18" max="18" width="12.7109375" style="23" customWidth="1"/>
+    <col min="19" max="19" width="18" style="23" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" style="23" customWidth="1"/>
+    <col min="21" max="16384" width="9.140625" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:25" ht="23.25">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29" t="s">
+        <v>1046</v>
+      </c>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29" t="s">
+        <v>1049</v>
+      </c>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="29"/>
+    </row>
+    <row r="4" spans="2:25" ht="18.75">
+      <c r="B4" s="25" t="s">
+        <v>1044</v>
+      </c>
+      <c r="E4" s="25" t="s">
+        <v>1043</v>
+      </c>
+      <c r="H4" s="25" t="s">
+        <v>1042</v>
+      </c>
+      <c r="O4" s="25" t="s">
+        <v>1047</v>
+      </c>
+      <c r="R4" s="25" t="s">
+        <v>1048</v>
+      </c>
+      <c r="U4" s="25" t="s">
+        <v>1042</v>
+      </c>
+    </row>
+    <row r="5" spans="2:25">
+      <c r="B5" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="F5" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="O5" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="P5" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="R5" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="S5" s="24" t="s">
+        <v>121</v>
+      </c>
+      <c r="U5" s="24" t="s">
+        <v>120</v>
+      </c>
+      <c r="V5" s="24" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="2:25" ht="15.75" customHeight="1" thickBot="1">
+      <c r="B6" s="28" t="s">
+        <v>478</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>479</v>
+      </c>
+      <c r="D6" s="26"/>
+      <c r="E6" s="28" t="s">
+        <v>480</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>481</v>
+      </c>
+      <c r="G6" s="26"/>
+      <c r="H6" s="28" t="s">
+        <v>474</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>475</v>
+      </c>
+      <c r="O6" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="P6" s="22" t="s">
+        <v>127</v>
+      </c>
+      <c r="Q6" s="26"/>
+      <c r="R6" s="9" t="s">
+        <v>175</v>
+      </c>
+      <c r="S6" s="10" t="s">
+        <v>176</v>
+      </c>
+      <c r="T6" s="26"/>
+      <c r="U6" s="28"/>
+      <c r="V6" s="28"/>
+    </row>
+    <row r="7" spans="2:25" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B7" s="28" t="s">
+        <v>488</v>
+      </c>
+      <c r="C7" s="28" t="s">
+        <v>489</v>
+      </c>
+      <c r="D7" s="26"/>
+      <c r="E7" s="28" t="s">
+        <v>482</v>
+      </c>
+      <c r="F7" s="28" t="s">
+        <v>483</v>
+      </c>
+      <c r="G7" s="26"/>
+      <c r="H7" s="28" t="s">
+        <v>476</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>477</v>
+      </c>
+      <c r="O7" s="22" t="s">
+        <v>128</v>
+      </c>
+      <c r="P7" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q7" s="26"/>
+      <c r="R7" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="S7" s="10" t="s">
+        <v>178</v>
+      </c>
+      <c r="T7" s="26"/>
+      <c r="U7" s="28"/>
+      <c r="V7" s="28"/>
+    </row>
+    <row r="8" spans="2:25" ht="18.75" customHeight="1" thickBot="1">
+      <c r="B8" s="28" t="s">
+        <v>539</v>
+      </c>
+      <c r="C8" s="28" t="s">
+        <v>540</v>
+      </c>
+      <c r="D8" s="26"/>
+      <c r="E8" s="28" t="s">
+        <v>484</v>
+      </c>
+      <c r="F8" s="28" t="s">
+        <v>485</v>
+      </c>
+      <c r="G8" s="26"/>
+      <c r="H8" s="28" t="s">
+        <v>537</v>
+      </c>
+      <c r="I8" s="28" t="s">
+        <v>538</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>1045</v>
+      </c>
+      <c r="O8" s="22" t="s">
+        <v>130</v>
+      </c>
+      <c r="P8" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q8" s="26"/>
+      <c r="R8" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="S8" s="10" t="s">
+        <v>179</v>
+      </c>
+      <c r="T8" s="26"/>
+      <c r="U8" s="28"/>
+      <c r="V8" s="28"/>
+      <c r="X8" s="27"/>
+    </row>
+    <row r="9" spans="2:25" ht="20.25" customHeight="1" thickBot="1">
+      <c r="B9" s="28" t="s">
+        <v>541</v>
+      </c>
+      <c r="C9" s="28" t="s">
+        <v>542</v>
+      </c>
+      <c r="D9" s="26"/>
+      <c r="E9" s="28" t="s">
+        <v>486</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>487</v>
+      </c>
+      <c r="G9" s="26"/>
+      <c r="H9" s="28" t="s">
+        <v>545</v>
+      </c>
+      <c r="I9" s="28" t="s">
+        <v>546</v>
+      </c>
+      <c r="K9" s="22" t="s">
+        <v>500</v>
+      </c>
+      <c r="L9" s="22" t="s">
+        <v>501</v>
+      </c>
+      <c r="O9" s="22" t="s">
+        <v>132</v>
+      </c>
+      <c r="P9" s="22" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q9" s="26"/>
+      <c r="R9" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="T9" s="26"/>
+      <c r="U9" s="28"/>
+      <c r="V9" s="28"/>
+      <c r="X9" s="22"/>
+      <c r="Y9" s="22"/>
+    </row>
+    <row r="10" spans="2:25">
+      <c r="B10" s="28" t="s">
+        <v>543</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>544</v>
+      </c>
+      <c r="D10" s="26"/>
+      <c r="E10" s="28" t="s">
+        <v>490</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>491</v>
+      </c>
+      <c r="G10" s="26"/>
+      <c r="H10" s="26"/>
+      <c r="I10" s="26"/>
+      <c r="K10" s="22" t="s">
+        <v>502</v>
+      </c>
+      <c r="L10" s="22" t="s">
+        <v>503</v>
+      </c>
+      <c r="O10" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="P10" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q10" s="26"/>
+      <c r="R10" s="28"/>
+      <c r="S10" s="28"/>
+      <c r="T10" s="26"/>
+      <c r="U10" s="26"/>
+      <c r="V10" s="26"/>
+      <c r="X10" s="22"/>
+      <c r="Y10" s="22"/>
+    </row>
+    <row r="11" spans="2:25" ht="20.25" customHeight="1">
+      <c r="B11" s="28" t="s">
+        <v>547</v>
+      </c>
+      <c r="C11" s="28" t="s">
+        <v>548</v>
+      </c>
+      <c r="D11" s="26"/>
+      <c r="E11" s="28" t="s">
+        <v>492</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>493</v>
+      </c>
+      <c r="G11" s="26"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="K11" s="22" t="s">
+        <v>504</v>
+      </c>
+      <c r="L11" s="22" t="s">
+        <v>505</v>
+      </c>
+      <c r="O11" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="P11" s="22" t="s">
+        <v>136</v>
+      </c>
+      <c r="Q11" s="26"/>
+      <c r="R11" s="28"/>
+      <c r="S11" s="28"/>
+      <c r="T11" s="26"/>
+      <c r="U11" s="26"/>
+      <c r="V11" s="26"/>
+      <c r="X11" s="22"/>
+      <c r="Y11" s="22"/>
+    </row>
+    <row r="12" spans="2:25" ht="18" customHeight="1">
+      <c r="B12" s="28" t="s">
+        <v>549</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>160</v>
+      </c>
+      <c r="D12" s="26"/>
+      <c r="E12" s="28" t="s">
+        <v>494</v>
+      </c>
+      <c r="F12" s="28" t="s">
+        <v>495</v>
+      </c>
+      <c r="G12" s="26"/>
+      <c r="H12" s="26"/>
+      <c r="I12" s="26"/>
+      <c r="K12" s="22" t="s">
+        <v>506</v>
+      </c>
+      <c r="L12" s="22" t="s">
+        <v>507</v>
+      </c>
+      <c r="O12" s="22" t="s">
+        <v>137</v>
+      </c>
+      <c r="P12" s="22" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q12" s="26"/>
+      <c r="R12" s="28"/>
+      <c r="S12" s="28"/>
+      <c r="T12" s="26"/>
+      <c r="U12" s="26"/>
+      <c r="V12" s="26"/>
+      <c r="X12" s="22"/>
+      <c r="Y12" s="22"/>
+    </row>
+    <row r="13" spans="2:25">
+      <c r="B13" s="28" t="s">
+        <v>553</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>554</v>
+      </c>
+      <c r="D13" s="26"/>
+      <c r="E13" s="28" t="s">
+        <v>496</v>
+      </c>
+      <c r="F13" s="28" t="s">
+        <v>497</v>
+      </c>
+      <c r="G13" s="26"/>
+      <c r="H13" s="26"/>
+      <c r="I13" s="26"/>
+      <c r="K13" s="22" t="s">
+        <v>510</v>
+      </c>
+      <c r="L13" s="22" t="s">
+        <v>511</v>
+      </c>
+      <c r="O13" s="22" t="s">
+        <v>139</v>
+      </c>
+      <c r="P13" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="Q13" s="26"/>
+      <c r="R13" s="28"/>
+      <c r="S13" s="28"/>
+      <c r="T13" s="26"/>
+      <c r="U13" s="26"/>
+      <c r="V13" s="26"/>
+      <c r="X13" s="22"/>
+      <c r="Y13" s="22"/>
+    </row>
+    <row r="14" spans="2:25">
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="28" t="s">
+        <v>520</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>521</v>
+      </c>
+      <c r="G14" s="26"/>
+      <c r="H14" s="26"/>
+      <c r="I14" s="26"/>
+      <c r="K14" s="22" t="s">
+        <v>512</v>
+      </c>
+      <c r="L14" s="22" t="s">
+        <v>513</v>
+      </c>
+      <c r="O14" s="22" t="s">
+        <v>141</v>
+      </c>
+      <c r="P14" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="Q14" s="26"/>
+      <c r="R14" s="28"/>
+      <c r="S14" s="28"/>
+      <c r="T14" s="26"/>
+      <c r="U14" s="26"/>
+      <c r="V14" s="26"/>
+      <c r="X14" s="22"/>
+      <c r="Y14" s="22"/>
+    </row>
+    <row r="15" spans="2:25">
+      <c r="B15" s="26"/>
+      <c r="C15" s="26"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="28" t="s">
+        <v>522</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>523</v>
+      </c>
+      <c r="G15" s="26"/>
+      <c r="H15" s="26"/>
+      <c r="I15" s="26"/>
+      <c r="K15" s="22" t="s">
+        <v>514</v>
+      </c>
+      <c r="L15" s="22" t="s">
+        <v>515</v>
+      </c>
+      <c r="O15" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="P15" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="Q15" s="26"/>
+      <c r="R15" s="28"/>
+      <c r="S15" s="28"/>
+      <c r="T15" s="26"/>
+      <c r="U15" s="26"/>
+      <c r="V15" s="26"/>
+      <c r="X15" s="22"/>
+      <c r="Y15" s="22"/>
+    </row>
+    <row r="16" spans="2:25" ht="15.75" thickBot="1">
+      <c r="B16" s="26"/>
+      <c r="C16" s="26"/>
+      <c r="D16" s="26"/>
+      <c r="E16" s="28" t="s">
+        <v>524</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>525</v>
+      </c>
+      <c r="G16" s="26"/>
+      <c r="H16" s="26"/>
+      <c r="I16" s="26"/>
+      <c r="K16" s="22" t="s">
+        <v>516</v>
+      </c>
+      <c r="L16" s="22" t="s">
+        <v>517</v>
+      </c>
+      <c r="O16" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="P16" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="Q16" s="26"/>
+      <c r="R16" s="9" t="s">
+        <v>197</v>
+      </c>
+      <c r="S16" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="T16" s="26"/>
+      <c r="U16" s="26"/>
+      <c r="V16" s="26"/>
+      <c r="X16" s="22"/>
+      <c r="Y16" s="22"/>
+    </row>
+    <row r="17" spans="2:25" ht="21.75" thickBot="1">
+      <c r="B17" s="26"/>
+      <c r="C17" s="26"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="28" t="s">
+        <v>526</v>
+      </c>
+      <c r="F17" s="28" t="s">
+        <v>527</v>
+      </c>
+      <c r="G17" s="26"/>
+      <c r="H17" s="26"/>
+      <c r="I17" s="26"/>
+      <c r="K17" s="22" t="s">
+        <v>498</v>
+      </c>
+      <c r="L17" s="22" t="s">
+        <v>499</v>
+      </c>
+      <c r="O17" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="P17" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="Q17" s="26"/>
+      <c r="R17" s="9" t="s">
+        <v>454</v>
+      </c>
+      <c r="S17" s="10" t="s">
+        <v>455</v>
+      </c>
+      <c r="T17" s="26"/>
+      <c r="U17" s="26"/>
+      <c r="V17" s="26"/>
+      <c r="X17" s="22"/>
+      <c r="Y17" s="22"/>
+    </row>
+    <row r="18" spans="2:25" ht="21.75" thickBot="1">
+      <c r="B18" s="26"/>
+      <c r="C18" s="26"/>
+      <c r="D18" s="26"/>
+      <c r="E18" s="28" t="s">
+        <v>529</v>
+      </c>
+      <c r="F18" s="28" t="s">
+        <v>530</v>
+      </c>
+      <c r="G18" s="26"/>
+      <c r="H18" s="26"/>
+      <c r="I18" s="26"/>
+      <c r="K18" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="L18" s="22" t="s">
+        <v>509</v>
+      </c>
+      <c r="O18" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="P18" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="Q18" s="26"/>
+      <c r="R18" s="9" t="s">
+        <v>456</v>
+      </c>
+      <c r="S18" s="10" t="s">
+        <v>457</v>
+      </c>
+      <c r="T18" s="26"/>
+      <c r="U18" s="26"/>
+      <c r="V18" s="26"/>
+      <c r="X18" s="22"/>
+      <c r="Y18" s="22"/>
+    </row>
+    <row r="19" spans="2:25" ht="21.75" thickBot="1">
+      <c r="B19" s="26"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="26"/>
+      <c r="E19" s="28" t="s">
+        <v>531</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>532</v>
+      </c>
+      <c r="G19" s="26"/>
+      <c r="H19" s="26"/>
+      <c r="I19" s="26"/>
+      <c r="K19" s="22" t="s">
+        <v>518</v>
+      </c>
+      <c r="L19" s="22" t="s">
+        <v>519</v>
+      </c>
+      <c r="O19" s="22" t="s">
+        <v>149</v>
+      </c>
+      <c r="P19" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q19" s="26"/>
+      <c r="R19" s="9" t="s">
+        <v>458</v>
+      </c>
+      <c r="S19" s="10" t="s">
+        <v>459</v>
+      </c>
+      <c r="T19" s="26"/>
+      <c r="U19" s="26"/>
+      <c r="V19" s="26"/>
+      <c r="X19" s="22"/>
+      <c r="Y19" s="22"/>
+    </row>
+    <row r="20" spans="2:25" ht="21.75" thickBot="1">
+      <c r="B20" s="26"/>
+      <c r="C20" s="26"/>
+      <c r="D20" s="26"/>
+      <c r="E20" s="28" t="s">
+        <v>533</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>534</v>
+      </c>
+      <c r="G20" s="26"/>
+      <c r="H20" s="26"/>
+      <c r="I20" s="26"/>
+      <c r="K20" s="22" t="s">
+        <v>528</v>
+      </c>
+      <c r="L20" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="O20" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="P20" s="22" t="s">
+        <v>151</v>
+      </c>
+      <c r="Q20" s="26"/>
+      <c r="R20" s="9" t="s">
+        <v>460</v>
+      </c>
+      <c r="S20" s="10" t="s">
+        <v>461</v>
+      </c>
+      <c r="T20" s="26"/>
+      <c r="U20" s="26"/>
+      <c r="V20" s="26"/>
+      <c r="X20" s="22"/>
+      <c r="Y20" s="22"/>
+    </row>
+    <row r="21" spans="2:25" ht="15.75" thickBot="1">
+      <c r="O21" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="P21" s="22" t="s">
+        <v>152</v>
+      </c>
+      <c r="R21" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="S21" s="10" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="22" spans="2:25" ht="15.75" thickBot="1">
+      <c r="O22" s="22" t="s">
+        <v>103</v>
+      </c>
+      <c r="P22" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="R22" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="S22" s="10" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="23" spans="2:25" ht="15.75" thickBot="1">
+      <c r="O23" s="22" t="s">
+        <v>154</v>
+      </c>
+      <c r="P23" s="22" t="s">
+        <v>155</v>
+      </c>
+      <c r="R23" s="9" t="s">
+        <v>631</v>
+      </c>
+      <c r="S23" s="10" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="24" spans="2:25" ht="15.75" thickBot="1">
+      <c r="O24" s="22" t="s">
+        <v>156</v>
+      </c>
+      <c r="P24" s="22" t="s">
+        <v>157</v>
+      </c>
+      <c r="R24" s="9" t="s">
+        <v>591</v>
+      </c>
+      <c r="S24" s="10" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="25" spans="2:25" ht="15.75" thickBot="1">
+      <c r="O25" s="22" t="s">
+        <v>158</v>
+      </c>
+      <c r="P25" s="22" t="s">
+        <v>159</v>
+      </c>
+      <c r="R25" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="S25" s="10" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="26" spans="2:25" ht="15.75" thickBot="1">
+      <c r="O26" s="22" t="s">
+        <v>160</v>
+      </c>
+      <c r="P26" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="R26" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="S26" s="10" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="27" spans="2:25" ht="15.75" thickBot="1">
+      <c r="O27" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="P27" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="R27" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="S27" s="8" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="28" spans="2:25" ht="21.75" thickBot="1">
+      <c r="O28" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="P28" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="R28" s="9" t="s">
+        <v>258</v>
+      </c>
+      <c r="S28" s="10" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="29" spans="2:25" ht="21.75" thickBot="1">
+      <c r="O29" s="22" t="s">
+        <v>105</v>
+      </c>
+      <c r="P29" s="22" t="s">
+        <v>165</v>
+      </c>
+      <c r="R29" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="S29" s="10" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="30" spans="2:25" ht="21.75" thickBot="1">
+      <c r="O30" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="P30" s="22" t="s">
+        <v>166</v>
+      </c>
+      <c r="R30" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="S30" s="10" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="31" spans="2:25" ht="15.75" thickBot="1">
+      <c r="O31" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="P31" s="22" t="s">
+        <v>167</v>
+      </c>
+      <c r="R31" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="S31" s="10" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="32" spans="2:25" ht="15.75" thickBot="1">
+      <c r="O32" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="P32" s="22" t="s">
+        <v>168</v>
+      </c>
+      <c r="R32" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="S32" s="10" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="33" spans="15:19" ht="15.75" thickBot="1">
+      <c r="O33" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="P33" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="R33" s="9" t="s">
+        <v>439</v>
+      </c>
+      <c r="S33" s="10" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="34" spans="15:19" ht="15.75" thickBot="1">
+      <c r="O34" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="P34" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="R34" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="S34" s="10" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="35" spans="15:19" ht="15.75" thickBot="1">
+      <c r="O35" s="22" t="s">
+        <v>86</v>
+      </c>
+      <c r="P35" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="R35" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="S35" s="10" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="36" spans="15:19">
+      <c r="O36" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="P36" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="37" spans="15:19">
+      <c r="O37" s="22" t="s">
+        <v>87</v>
+      </c>
+      <c r="P37" s="22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added sorted PCI express USB
</commit_message>
<xml_diff>
--- a/Excel Sheet/Southbridge.xlsx
+++ b/Excel Sheet/Southbridge.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2751" uniqueCount="1062">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2975" uniqueCount="1072">
   <si>
     <t>A</t>
   </si>
@@ -3202,13 +3202,43 @@
   </si>
   <si>
     <t>Sleep/other</t>
+  </si>
+  <si>
+    <t>USB</t>
+  </si>
+  <si>
+    <t>Differentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> OC Indicators</t>
+  </si>
+  <si>
+    <t>Pwr</t>
+  </si>
+  <si>
+    <t>Clk Signals</t>
+  </si>
+  <si>
+    <t>DMI</t>
+  </si>
+  <si>
+    <t>Impedence</t>
+  </si>
+  <si>
+    <t>PCI Express</t>
+  </si>
+  <si>
+    <t>GLAN Interface</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="9">
+  <fonts count="10">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3275,6 +3305,13 @@
       <color rgb="FFFF0000"/>
       <name val="Verdana"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="7">
@@ -3446,7 +3483,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3525,6 +3562,19 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -5759,8 +5809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D677"/>
   <sheetViews>
-    <sheetView topLeftCell="A423" workbookViewId="0">
-      <selection activeCell="F438" sqref="F438"/>
+    <sheetView topLeftCell="A112" workbookViewId="0">
+      <selection activeCell="F121" sqref="F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6121,18 +6171,18 @@
       </c>
     </row>
     <row r="45" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A45" s="9" t="s">
+      <c r="C45" s="9" t="s">
         <v>110</v>
       </c>
-      <c r="B45" s="10" t="s">
+      <c r="D45" s="10" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="46" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A46" s="9" t="s">
+      <c r="C46" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="D46" s="10" t="s">
         <v>193</v>
       </c>
     </row>
@@ -6152,7 +6202,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="15.75" thickBot="1">
+    <row r="49" spans="3:4" ht="15.75" thickBot="1">
       <c r="C49" s="9" t="s">
         <v>197</v>
       </c>
@@ -6160,163 +6210,163 @@
         <v>198</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A50" s="9" t="s">
+    <row r="50" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C50" s="9" t="s">
         <v>199</v>
       </c>
-      <c r="B50" s="10" t="s">
+      <c r="D50" s="10" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A51" s="9" t="s">
+    <row r="51" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C51" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="D51" s="10" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A52" s="9" t="s">
+    <row r="52" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C52" s="9" t="s">
         <v>203</v>
       </c>
-      <c r="B52" s="10" t="s">
+      <c r="D52" s="10" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A53" s="9" t="s">
+    <row r="53" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C53" s="9" t="s">
         <v>205</v>
       </c>
-      <c r="B53" s="10" t="s">
+      <c r="D53" s="10" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A54" s="9" t="s">
+    <row r="54" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C54" s="9" t="s">
         <v>207</v>
       </c>
-      <c r="B54" s="10" t="s">
+      <c r="D54" s="10" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A55" s="9" t="s">
+    <row r="55" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C55" s="9" t="s">
         <v>209</v>
       </c>
-      <c r="B55" s="10" t="s">
+      <c r="D55" s="10" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A56" s="9" t="s">
+    <row r="56" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C56" s="9" t="s">
         <v>211</v>
       </c>
-      <c r="B56" s="10" t="s">
+      <c r="D56" s="10" t="s">
         <v>212</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A57" s="9" t="s">
+    <row r="57" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C57" s="9" t="s">
         <v>213</v>
       </c>
-      <c r="B57" s="10" t="s">
+      <c r="D57" s="10" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A58" s="9" t="s">
+    <row r="58" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C58" s="9" t="s">
         <v>215</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="D58" s="10" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A59" s="9" t="s">
+    <row r="59" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C59" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="B59" s="10" t="s">
+      <c r="D59" s="10" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A60" s="9" t="s">
+    <row r="60" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C60" s="9" t="s">
         <v>219</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="D60" s="10" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A61" s="9" t="s">
+    <row r="61" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C61" s="9" t="s">
         <v>221</v>
       </c>
-      <c r="B61" s="10" t="s">
+      <c r="D61" s="10" t="s">
         <v>222</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A62" s="9" t="s">
+    <row r="62" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C62" s="9" t="s">
         <v>223</v>
       </c>
-      <c r="B62" s="10" t="s">
+      <c r="D62" s="10" t="s">
         <v>224</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A63" s="9" t="s">
+    <row r="63" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C63" s="9" t="s">
         <v>225</v>
       </c>
-      <c r="B63" s="10" t="s">
+      <c r="D63" s="10" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A64" s="9" t="s">
+    <row r="64" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C64" s="9" t="s">
         <v>227</v>
       </c>
-      <c r="B64" s="10" t="s">
+      <c r="D64" s="10" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="65" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A65" s="9" t="s">
+      <c r="C65" s="9" t="s">
         <v>229</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="D65" s="10" t="s">
         <v>230</v>
       </c>
     </row>
     <row r="66" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A66" s="9" t="s">
+      <c r="C66" s="9" t="s">
         <v>231</v>
       </c>
-      <c r="B66" s="10" t="s">
+      <c r="D66" s="10" t="s">
         <v>232</v>
       </c>
     </row>
     <row r="67" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A67" s="9" t="s">
+      <c r="C67" s="9" t="s">
         <v>233</v>
       </c>
-      <c r="B67" s="10" t="s">
+      <c r="D67" s="10" t="s">
         <v>234</v>
       </c>
     </row>
     <row r="68" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A68" s="9" t="s">
+      <c r="C68" s="9" t="s">
         <v>235</v>
       </c>
-      <c r="B68" s="10" t="s">
+      <c r="D68" s="10" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="69" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A69" s="9" t="s">
+      <c r="C69" s="9" t="s">
         <v>236</v>
       </c>
-      <c r="B69" s="10" t="s">
+      <c r="D69" s="10" t="s">
         <v>48</v>
       </c>
     </row>
@@ -6376,27 +6426,27 @@
         <v>250</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A77" s="9" t="s">
+    <row r="77" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C77" s="9" t="s">
         <v>251</v>
       </c>
-      <c r="B77" s="10" t="s">
+      <c r="D77" s="10" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A78" s="9" t="s">
+    <row r="78" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C78" s="9" t="s">
         <v>253</v>
       </c>
-      <c r="B78" s="10" t="s">
+      <c r="D78" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A79" s="9" t="s">
+    <row r="79" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C79" s="9" t="s">
         <v>255</v>
       </c>
-      <c r="B79" s="10" t="s">
+      <c r="D79" s="10" t="s">
         <v>256</v>
       </c>
     </row>
@@ -6712,59 +6762,59 @@
         <v>322</v>
       </c>
     </row>
-    <row r="119" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A119" s="7" t="s">
+    <row r="119" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C119" s="7" t="s">
         <v>323</v>
       </c>
-      <c r="B119" s="8" t="s">
+      <c r="D119" s="8" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="120" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A120" s="9" t="s">
+    <row r="120" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C120" s="30" t="s">
         <v>325</v>
       </c>
-      <c r="B120" s="10" t="s">
+      <c r="D120" s="31" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="121" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A121" s="9" t="s">
+    <row r="121" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C121" s="30" t="s">
         <v>327</v>
       </c>
-      <c r="B121" s="10" t="s">
+      <c r="D121" s="31" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="122" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A122" s="9" t="s">
+    <row r="122" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C122" s="30" t="s">
         <v>329</v>
       </c>
-      <c r="B122" s="10" t="s">
+      <c r="D122" s="31" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="123" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A123" s="9" t="s">
+    <row r="123" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C123" s="30" t="s">
         <v>331</v>
       </c>
-      <c r="B123" s="10" t="s">
+      <c r="D123" s="31" t="s">
         <v>332</v>
       </c>
     </row>
-    <row r="124" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A124" s="9" t="s">
+    <row r="124" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C124" s="30" t="s">
         <v>333</v>
       </c>
-      <c r="B124" s="10" t="s">
+      <c r="D124" s="31" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="125" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A125" s="9" t="s">
+    <row r="125" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C125" s="30" t="s">
         <v>335</v>
       </c>
-      <c r="B125" s="10" t="s">
+      <c r="D125" s="31" t="s">
         <v>336</v>
       </c>
     </row>
@@ -6816,99 +6866,99 @@
         <v>348</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A132" s="9" t="s">
+    <row r="132" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C132" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="B132" s="10" t="s">
+      <c r="D132" s="10" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A133" s="9" t="s">
+    <row r="133" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C133" s="9" t="s">
         <v>351</v>
       </c>
-      <c r="B133" s="10" t="s">
+      <c r="D133" s="10" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="134" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A134" s="9" t="s">
+    <row r="134" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C134" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="B134" s="10" t="s">
+      <c r="D134" s="10" t="s">
         <v>354</v>
       </c>
     </row>
-    <row r="135" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A135" s="9" t="s">
+    <row r="135" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C135" s="9" t="s">
         <v>355</v>
       </c>
-      <c r="B135" s="10" t="s">
+      <c r="D135" s="10" t="s">
         <v>356</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A136" s="9" t="s">
+    <row r="136" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C136" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="B136" s="10" t="s">
+      <c r="D136" s="10" t="s">
         <v>358</v>
       </c>
     </row>
-    <row r="137" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A137" s="9" t="s">
+    <row r="137" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C137" s="9" t="s">
         <v>359</v>
       </c>
-      <c r="B137" s="10" t="s">
+      <c r="D137" s="10" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="138" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A138" s="9" t="s">
+    <row r="138" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C138" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="B138" s="10" t="s">
+      <c r="D138" s="10" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="139" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A139" s="9" t="s">
+    <row r="139" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C139" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="B139" s="10" t="s">
+      <c r="D139" s="10" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="140" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A140" s="9" t="s">
+    <row r="140" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C140" s="9" t="s">
         <v>365</v>
       </c>
-      <c r="B140" s="10" t="s">
+      <c r="D140" s="10" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="141" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A141" s="9" t="s">
+    <row r="141" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C141" s="9" t="s">
         <v>367</v>
       </c>
-      <c r="B141" s="10" t="s">
+      <c r="D141" s="10" t="s">
         <v>368</v>
       </c>
     </row>
-    <row r="142" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A142" s="9" t="s">
+    <row r="142" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C142" s="9" t="s">
         <v>369</v>
       </c>
-      <c r="B142" s="10" t="s">
+      <c r="D142" s="10" t="s">
         <v>370</v>
       </c>
     </row>
-    <row r="143" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A143" s="9" t="s">
+    <row r="143" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C143" s="9" t="s">
         <v>371</v>
       </c>
-      <c r="B143" s="10" t="s">
+      <c r="D143" s="10" t="s">
         <v>372</v>
       </c>
     </row>
@@ -6945,98 +6995,98 @@
       </c>
     </row>
     <row r="148" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A148" s="9" t="s">
+      <c r="C148" s="9" t="s">
         <v>378</v>
       </c>
-      <c r="B148" s="10" t="s">
+      <c r="D148" s="10" t="s">
         <v>379</v>
       </c>
     </row>
     <row r="149" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A149" s="9" t="s">
+      <c r="C149" s="9" t="s">
         <v>380</v>
       </c>
-      <c r="B149" s="10" t="s">
+      <c r="D149" s="10" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="150" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A150" s="9" t="s">
+      <c r="C150" s="9" t="s">
         <v>382</v>
       </c>
-      <c r="B150" s="10" t="s">
+      <c r="D150" s="10" t="s">
         <v>383</v>
       </c>
     </row>
     <row r="151" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A151" s="9" t="s">
+      <c r="C151" s="9" t="s">
         <v>384</v>
       </c>
-      <c r="B151" s="10" t="s">
+      <c r="D151" s="10" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="152" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A152" s="9" t="s">
+      <c r="C152" s="9" t="s">
         <v>386</v>
       </c>
-      <c r="B152" s="10" t="s">
+      <c r="D152" s="10" t="s">
         <v>387</v>
       </c>
     </row>
-    <row r="153" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A153" s="9" t="s">
+    <row r="153" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C153" s="9" t="s">
         <v>388</v>
       </c>
-      <c r="B153" s="10" t="s">
+      <c r="D153" s="10" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="154" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A154" s="9" t="s">
+      <c r="C154" s="9" t="s">
         <v>390</v>
       </c>
-      <c r="B154" s="10" t="s">
+      <c r="D154" s="10" t="s">
         <v>391</v>
       </c>
     </row>
     <row r="155" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A155" s="9" t="s">
+      <c r="C155" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="B155" s="10" t="s">
+      <c r="D155" s="10" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="156" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A156" s="9" t="s">
+      <c r="C156" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="B156" s="10" t="s">
+      <c r="D156" s="10" t="s">
         <v>395</v>
       </c>
     </row>
     <row r="157" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A157" s="7" t="s">
+      <c r="C157" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="B157" s="8" t="s">
+      <c r="D157" s="8" t="s">
         <v>397</v>
       </c>
     </row>
     <row r="158" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A158" s="9" t="s">
+      <c r="C158" s="9" t="s">
         <v>398</v>
       </c>
-      <c r="B158" s="10" t="s">
+      <c r="D158" s="10" t="s">
         <v>399</v>
       </c>
     </row>
-    <row r="159" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A159" s="9" t="s">
+    <row r="159" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C159" s="9" t="s">
         <v>400</v>
       </c>
-      <c r="B159" s="10" t="s">
+      <c r="D159" s="10" t="s">
         <v>401</v>
       </c>
     </row>
@@ -7048,103 +7098,103 @@
         <v>402</v>
       </c>
     </row>
-    <row r="161" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A161" s="9" t="s">
+    <row r="161" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C161" s="9" t="s">
         <v>403</v>
       </c>
-      <c r="B161" s="10" t="s">
+      <c r="D161" s="10" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="162" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A162" s="9" t="s">
+    <row r="162" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C162" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="B162" s="10" t="s">
+      <c r="D162" s="10" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="163" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A163" s="9" t="s">
+    <row r="163" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C163" s="9" t="s">
         <v>407</v>
       </c>
-      <c r="B163" s="10" t="s">
+      <c r="D163" s="10" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="164" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A164" s="9" t="s">
+    <row r="164" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C164" s="9" t="s">
         <v>409</v>
       </c>
-      <c r="B164" s="10" t="s">
+      <c r="D164" s="10" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="165" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A165" s="9" t="s">
+    <row r="165" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C165" s="9" t="s">
         <v>411</v>
       </c>
-      <c r="B165" s="10" t="s">
+      <c r="D165" s="10" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="166" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A166" s="9" t="s">
+    <row r="166" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C166" s="9" t="s">
         <v>413</v>
       </c>
-      <c r="B166" s="10" t="s">
+      <c r="D166" s="10" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="167" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A167" s="9" t="s">
+    <row r="167" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C167" s="9" t="s">
         <v>415</v>
       </c>
-      <c r="B167" s="10" t="s">
+      <c r="D167" s="10" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="168" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A168" s="9" t="s">
+    <row r="168" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C168" s="9" t="s">
         <v>417</v>
       </c>
-      <c r="B168" s="10" t="s">
+      <c r="D168" s="10" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="169" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A169" s="9" t="s">
+    <row r="169" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C169" s="9" t="s">
         <v>419</v>
       </c>
-      <c r="B169" s="10" t="s">
+      <c r="D169" s="10" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="170" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A170" s="9" t="s">
+    <row r="170" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C170" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="B170" s="10" t="s">
+      <c r="D170" s="10" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="171" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A171" s="9" t="s">
+    <row r="171" spans="1:4" ht="15.75" thickBot="1">
+      <c r="C171" s="9" t="s">
         <v>423</v>
       </c>
-      <c r="B171" s="10" t="s">
+      <c r="D171" s="10" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="172" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A172" s="9" t="s">
+    <row r="172" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C172" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="B172" s="10" t="s">
+      <c r="D172" s="10" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="173" spans="1:2" ht="15.75" thickBot="1">
+    <row r="173" spans="1:4" ht="15.75" thickBot="1">
       <c r="A173" s="9" t="s">
         <v>107</v>
       </c>
@@ -7152,7 +7202,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="174" spans="1:2" ht="15.75" thickBot="1">
+    <row r="174" spans="1:4" ht="15.75" thickBot="1">
       <c r="A174" s="9" t="s">
         <v>43</v>
       </c>
@@ -7160,7 +7210,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="175" spans="1:2" ht="15.75" thickBot="1">
+    <row r="175" spans="1:4" ht="15.75" thickBot="1">
       <c r="A175" s="9" t="s">
         <v>47</v>
       </c>
@@ -7168,7 +7218,7 @@
         <v>429</v>
       </c>
     </row>
-    <row r="176" spans="1:2" ht="15.75" thickBot="1">
+    <row r="176" spans="1:4" ht="15.75" thickBot="1">
       <c r="A176" s="9" t="s">
         <v>44</v>
       </c>
@@ -7337,18 +7387,18 @@
       </c>
     </row>
     <row r="197" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A197" s="9" t="s">
+      <c r="C197" s="9" t="s">
         <v>468</v>
       </c>
-      <c r="B197" s="10" t="s">
+      <c r="D197" s="10" t="s">
         <v>469</v>
       </c>
     </row>
     <row r="198" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A198" s="9" t="s">
+      <c r="C198" s="9" t="s">
         <v>470</v>
       </c>
-      <c r="B198" s="10" t="s">
+      <c r="D198" s="10" t="s">
         <v>471</v>
       </c>
     </row>
@@ -8017,246 +8067,246 @@
       </c>
     </row>
     <row r="282" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A282" s="9" t="s">
+      <c r="C282" s="9" t="s">
         <v>633</v>
       </c>
-      <c r="B282" s="10" t="s">
+      <c r="D282" s="10" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="283" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A283" s="9" t="s">
+      <c r="C283" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="B283" s="10" t="s">
+      <c r="D283" s="10" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="284" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A284" s="9" t="s">
+      <c r="C284" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="B284" s="10" t="s">
+      <c r="D284" s="10" t="s">
         <v>634</v>
       </c>
     </row>
     <row r="285" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A285" s="9" t="s">
+      <c r="C285" s="9" t="s">
         <v>81</v>
       </c>
-      <c r="B285" s="10" t="s">
+      <c r="D285" s="10" t="s">
         <v>635</v>
       </c>
     </row>
     <row r="286" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A286" s="9" t="s">
+      <c r="C286" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B286" s="10" t="s">
+      <c r="D286" s="10" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="287" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A287" s="9" t="s">
+      <c r="C287" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="B287" s="10" t="s">
+      <c r="D287" s="10" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="288" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A288" s="9" t="s">
+      <c r="C288" s="9" t="s">
         <v>636</v>
       </c>
-      <c r="B288" s="10" t="s">
+      <c r="D288" s="10" t="s">
         <v>637</v>
       </c>
     </row>
-    <row r="289" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A289" s="9" t="s">
+    <row r="289" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C289" s="9" t="s">
         <v>117</v>
       </c>
-      <c r="B289" s="10" t="s">
+      <c r="D289" s="10" t="s">
         <v>638</v>
       </c>
     </row>
-    <row r="290" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A290" s="9" t="s">
+    <row r="290" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C290" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="B290" s="10" t="s">
+      <c r="D290" s="10" t="s">
         <v>639</v>
       </c>
     </row>
-    <row r="291" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A291" s="9" t="s">
+    <row r="291" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C291" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="B291" s="10" t="s">
+      <c r="D291" s="10" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="292" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A292" s="9" t="s">
+    <row r="292" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C292" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="B292" s="10" t="s">
+      <c r="D292" s="10" t="s">
         <v>641</v>
       </c>
     </row>
-    <row r="293" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A293" s="9" t="s">
+    <row r="293" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C293" s="9" t="s">
         <v>78</v>
       </c>
-      <c r="B293" s="10" t="s">
+      <c r="D293" s="10" t="s">
         <v>642</v>
       </c>
     </row>
-    <row r="294" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A294" s="9" t="s">
+    <row r="294" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C294" s="9" t="s">
         <v>643</v>
       </c>
-      <c r="B294" s="10" t="s">
+      <c r="D294" s="10" t="s">
         <v>644</v>
       </c>
     </row>
-    <row r="295" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A295" s="9" t="s">
+    <row r="295" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C295" s="9" t="s">
         <v>116</v>
       </c>
-      <c r="B295" s="10" t="s">
+      <c r="D295" s="10" t="s">
         <v>645</v>
       </c>
     </row>
-    <row r="296" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A296" s="9" t="s">
+    <row r="296" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C296" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B296" s="10" t="s">
+      <c r="D296" s="10" t="s">
         <v>646</v>
       </c>
     </row>
-    <row r="297" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A297" s="9" t="s">
+    <row r="297" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C297" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="B297" s="10" t="s">
+      <c r="D297" s="10" t="s">
         <v>647</v>
       </c>
     </row>
-    <row r="298" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A298" s="9" t="s">
+    <row r="298" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C298" s="9" t="s">
         <v>60</v>
       </c>
-      <c r="B298" s="10" t="s">
+      <c r="D298" s="10" t="s">
         <v>648</v>
       </c>
     </row>
-    <row r="299" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A299" s="9" t="s">
+    <row r="299" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C299" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="B299" s="10" t="s">
+      <c r="D299" s="10" t="s">
         <v>649</v>
       </c>
     </row>
-    <row r="300" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A300" s="9" t="s">
+    <row r="300" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C300" s="9" t="s">
         <v>650</v>
       </c>
-      <c r="B300" s="10" t="s">
+      <c r="D300" s="10" t="s">
         <v>651</v>
       </c>
     </row>
-    <row r="301" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A301" s="9" t="s">
+    <row r="301" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C301" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B301" s="10" t="s">
+      <c r="D301" s="10" t="s">
         <v>652</v>
       </c>
     </row>
-    <row r="302" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A302" s="9" t="s">
+    <row r="302" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C302" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="B302" s="10" t="s">
+      <c r="D302" s="10" t="s">
         <v>653</v>
       </c>
     </row>
-    <row r="303" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A303" s="9" t="s">
+    <row r="303" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C303" s="9" t="s">
         <v>95</v>
       </c>
-      <c r="B303" s="10" t="s">
+      <c r="D303" s="10" t="s">
         <v>654</v>
       </c>
     </row>
-    <row r="304" spans="1:2" ht="15.75" thickBot="1">
-      <c r="A304" s="9" t="s">
+    <row r="304" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C304" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="B304" s="10" t="s">
+      <c r="D304" s="10" t="s">
         <v>655</v>
       </c>
     </row>
-    <row r="305" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A305" s="9" t="s">
+    <row r="305" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C305" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="B305" s="10" t="s">
+      <c r="D305" s="10" t="s">
         <v>656</v>
       </c>
     </row>
-    <row r="306" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A306" s="9" t="s">
+    <row r="306" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C306" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="B306" s="10" t="s">
+      <c r="D306" s="10" t="s">
         <v>657</v>
       </c>
     </row>
-    <row r="307" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A307" s="9" t="s">
+    <row r="307" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C307" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B307" s="10" t="s">
+      <c r="D307" s="10" t="s">
         <v>658</v>
       </c>
     </row>
-    <row r="308" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A308" s="7" t="s">
+    <row r="308" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C308" s="32" t="s">
         <v>659</v>
       </c>
-      <c r="B308" s="8" t="s">
+      <c r="D308" s="33" t="s">
         <v>660</v>
       </c>
     </row>
-    <row r="309" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A309" s="9" t="s">
+    <row r="309" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C309" s="30" t="s">
         <v>659</v>
       </c>
-      <c r="B309" s="10" t="s">
+      <c r="D309" s="31" t="s">
         <v>661</v>
       </c>
     </row>
-    <row r="310" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A310" s="9" t="s">
+    <row r="310" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C310" s="30" t="s">
         <v>662</v>
       </c>
-      <c r="B310" s="10" t="s">
+      <c r="D310" s="31" t="s">
         <v>663</v>
       </c>
     </row>
-    <row r="311" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A311" s="9" t="s">
+    <row r="311" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C311" s="30" t="s">
         <v>63</v>
       </c>
-      <c r="B311" s="10" t="s">
+      <c r="D311" s="31" t="s">
         <v>664</v>
       </c>
     </row>
-    <row r="312" spans="1:4" ht="15.75" thickBot="1">
+    <row r="312" spans="3:4" ht="15.75" thickBot="1">
       <c r="C312" s="9" t="s">
         <v>31</v>
       </c>
@@ -8264,7 +8314,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="313" spans="1:4" ht="15.75" thickBot="1">
+    <row r="313" spans="3:4" ht="15.75" thickBot="1">
       <c r="C313" s="9" t="s">
         <v>31</v>
       </c>
@@ -8272,7 +8322,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="314" spans="1:4" ht="15.75" thickBot="1">
+    <row r="314" spans="3:4" ht="15.75" thickBot="1">
       <c r="C314" s="9" t="s">
         <v>31</v>
       </c>
@@ -8280,7 +8330,7 @@
         <v>667</v>
       </c>
     </row>
-    <row r="315" spans="1:4" ht="15.75" thickBot="1">
+    <row r="315" spans="3:4" ht="15.75" thickBot="1">
       <c r="C315" s="9" t="s">
         <v>31</v>
       </c>
@@ -8288,7 +8338,7 @@
         <v>668</v>
       </c>
     </row>
-    <row r="316" spans="1:4" ht="15.75" thickBot="1">
+    <row r="316" spans="3:4" ht="15.75" thickBot="1">
       <c r="C316" s="9" t="s">
         <v>31</v>
       </c>
@@ -8296,7 +8346,7 @@
         <v>669</v>
       </c>
     </row>
-    <row r="317" spans="1:4" ht="15.75" thickBot="1">
+    <row r="317" spans="3:4" ht="15.75" thickBot="1">
       <c r="C317" s="9" t="s">
         <v>31</v>
       </c>
@@ -8304,7 +8354,7 @@
         <v>670</v>
       </c>
     </row>
-    <row r="318" spans="1:4" ht="15.75" thickBot="1">
+    <row r="318" spans="3:4" ht="15.75" thickBot="1">
       <c r="C318" s="9" t="s">
         <v>31</v>
       </c>
@@ -8312,7 +8362,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="319" spans="1:4" ht="15.75" thickBot="1">
+    <row r="319" spans="3:4" ht="15.75" thickBot="1">
       <c r="C319" s="9" t="s">
         <v>31</v>
       </c>
@@ -8320,7 +8370,7 @@
         <v>672</v>
       </c>
     </row>
-    <row r="320" spans="1:4" ht="15.75" thickBot="1">
+    <row r="320" spans="3:4" ht="15.75" thickBot="1">
       <c r="C320" s="9" t="s">
         <v>31</v>
       </c>
@@ -9480,7 +9530,7 @@
         <v>824</v>
       </c>
     </row>
-    <row r="465" spans="1:4" ht="21.75" thickBot="1">
+    <row r="465" spans="3:4" ht="21.75" thickBot="1">
       <c r="C465" s="9" t="s">
         <v>58</v>
       </c>
@@ -9488,7 +9538,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="466" spans="1:4" ht="21.75" thickBot="1">
+    <row r="466" spans="3:4" ht="21.75" thickBot="1">
       <c r="C466" s="9" t="s">
         <v>58</v>
       </c>
@@ -9496,7 +9546,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="467" spans="1:4" ht="21.75" thickBot="1">
+    <row r="467" spans="3:4" ht="21.75" thickBot="1">
       <c r="C467" s="9" t="s">
         <v>58</v>
       </c>
@@ -9504,7 +9554,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="468" spans="1:4" ht="21.75" thickBot="1">
+    <row r="468" spans="3:4" ht="21.75" thickBot="1">
       <c r="C468" s="9" t="s">
         <v>58</v>
       </c>
@@ -9512,7 +9562,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="469" spans="1:4" ht="21.75" thickBot="1">
+    <row r="469" spans="3:4" ht="21.75" thickBot="1">
       <c r="C469" s="9" t="s">
         <v>58</v>
       </c>
@@ -9520,7 +9570,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="470" spans="1:4" ht="21.75" thickBot="1">
+    <row r="470" spans="3:4" ht="21.75" thickBot="1">
       <c r="C470" s="9" t="s">
         <v>58</v>
       </c>
@@ -9528,7 +9578,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="471" spans="1:4" ht="21.75" thickBot="1">
+    <row r="471" spans="3:4" ht="21.75" thickBot="1">
       <c r="C471" s="9" t="s">
         <v>58</v>
       </c>
@@ -9536,7 +9586,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="472" spans="1:4" ht="21.75" thickBot="1">
+    <row r="472" spans="3:4" ht="21.75" thickBot="1">
       <c r="C472" s="9" t="s">
         <v>58</v>
       </c>
@@ -9544,7 +9594,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="473" spans="1:4" ht="21.75" thickBot="1">
+    <row r="473" spans="3:4" ht="21.75" thickBot="1">
       <c r="C473" s="9" t="s">
         <v>58</v>
       </c>
@@ -9552,7 +9602,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="474" spans="1:4" ht="21.75" thickBot="1">
+    <row r="474" spans="3:4" ht="21.75" thickBot="1">
       <c r="C474" s="9" t="s">
         <v>58</v>
       </c>
@@ -9560,7 +9610,7 @@
         <v>834</v>
       </c>
     </row>
-    <row r="475" spans="1:4" ht="21.75" thickBot="1">
+    <row r="475" spans="3:4" ht="21.75" thickBot="1">
       <c r="C475" s="9" t="s">
         <v>58</v>
       </c>
@@ -9568,23 +9618,23 @@
         <v>835</v>
       </c>
     </row>
-    <row r="476" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A476" s="9" t="s">
+    <row r="476" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C476" s="30" t="s">
         <v>836</v>
       </c>
-      <c r="B476" s="10" t="s">
+      <c r="D476" s="31" t="s">
         <v>837</v>
       </c>
     </row>
-    <row r="477" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A477" s="9" t="s">
+    <row r="477" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C477" s="30" t="s">
         <v>838</v>
       </c>
-      <c r="B477" s="10" t="s">
+      <c r="D477" s="31" t="s">
         <v>839</v>
       </c>
     </row>
-    <row r="478" spans="1:4" ht="21.75" thickBot="1">
+    <row r="478" spans="3:4" ht="21.75" thickBot="1">
       <c r="C478" s="9" t="s">
         <v>840</v>
       </c>
@@ -9592,7 +9642,7 @@
         <v>841</v>
       </c>
     </row>
-    <row r="479" spans="1:4" ht="15.75" thickBot="1">
+    <row r="479" spans="3:4" ht="15.75" thickBot="1">
       <c r="C479" s="9" t="s">
         <v>30</v>
       </c>
@@ -9600,7 +9650,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="480" spans="1:4" ht="15.75" thickBot="1">
+    <row r="480" spans="3:4" ht="15.75" thickBot="1">
       <c r="C480" s="9" t="s">
         <v>30</v>
       </c>
@@ -11186,15 +11236,16 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:BO106"/>
+  <dimension ref="B2:DA106"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="BC24" sqref="BC24"/>
+    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="CW14" sqref="CW14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11225,10 +11276,12 @@
     <col min="41" max="41" width="16.140625" style="24" customWidth="1"/>
     <col min="42" max="62" width="9.140625" style="24"/>
     <col min="63" max="63" width="12.140625" style="24" customWidth="1"/>
-    <col min="64" max="16384" width="9.140625" style="24"/>
+    <col min="64" max="69" width="9.140625" style="24"/>
+    <col min="70" max="70" width="12.7109375" style="24" customWidth="1"/>
+    <col min="71" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:67" ht="23.25">
+    <row r="2" spans="2:105" ht="23.25">
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -11308,8 +11361,45 @@
       </c>
       <c r="BN2" s="26"/>
       <c r="BO2" s="26"/>
-    </row>
-    <row r="4" spans="2:67" ht="18.75">
+      <c r="BR2" s="26"/>
+      <c r="BS2" s="26"/>
+      <c r="BT2" s="26"/>
+      <c r="BU2" s="26" t="s">
+        <v>1062</v>
+      </c>
+      <c r="BV2" s="26"/>
+      <c r="BW2" s="26"/>
+      <c r="BX2" s="26"/>
+      <c r="BY2" s="26"/>
+      <c r="CB2" s="26" t="s">
+        <v>1066</v>
+      </c>
+      <c r="CC2" s="26"/>
+      <c r="CD2" s="26"/>
+      <c r="CG2" s="26"/>
+      <c r="CH2" s="26"/>
+      <c r="CI2" s="26"/>
+      <c r="CJ2" s="26" t="s">
+        <v>1067</v>
+      </c>
+      <c r="CK2" s="26"/>
+      <c r="CN2" s="26" t="s">
+        <v>1069</v>
+      </c>
+      <c r="CO2" s="26"/>
+      <c r="CP2" s="26"/>
+      <c r="CS2" s="26"/>
+      <c r="CT2" s="26"/>
+      <c r="CU2" s="26"/>
+      <c r="CV2" s="26" t="s">
+        <v>1070</v>
+      </c>
+      <c r="CW2" s="26"/>
+      <c r="CX2" s="26"/>
+      <c r="CY2" s="26"/>
+      <c r="CZ2" s="26"/>
+    </row>
+    <row r="4" spans="2:105" ht="18.75">
       <c r="B4" s="23" t="s">
         <v>1044</v>
       </c>
@@ -11347,8 +11437,39 @@
       <c r="AX4" s="23"/>
       <c r="BA4" s="23"/>
       <c r="BD4" s="23"/>
-    </row>
-    <row r="5" spans="2:67">
+      <c r="BR4" s="23" t="s">
+        <v>1063</v>
+      </c>
+      <c r="BU4" s="23" t="s">
+        <v>1065</v>
+      </c>
+      <c r="BX4" s="23" t="s">
+        <v>1064</v>
+      </c>
+      <c r="CB4" s="23" t="s">
+        <v>1063</v>
+      </c>
+      <c r="CE4" s="23"/>
+      <c r="CG4" s="23" t="s">
+        <v>1068</v>
+      </c>
+      <c r="CJ4" s="23" t="s">
+        <v>1063</v>
+      </c>
+      <c r="CM4" s="23"/>
+      <c r="CN4" s="23" t="s">
+        <v>1063</v>
+      </c>
+      <c r="CQ4" s="23"/>
+      <c r="CS4" s="23" t="s">
+        <v>1071</v>
+      </c>
+      <c r="CV4" s="23" t="s">
+        <v>1068</v>
+      </c>
+      <c r="CY4" s="23"/>
+    </row>
+    <row r="5" spans="2:105">
       <c r="B5" s="22" t="s">
         <v>120</v>
       </c>
@@ -11465,8 +11586,69 @@
       <c r="BN5" s="22" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="6" spans="2:67" ht="15.75" customHeight="1">
+      <c r="BR5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="BS5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="BU5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="BV5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="BX5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="BY5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="CB5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="CC5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="CE5" s="22"/>
+      <c r="CF5" s="22"/>
+      <c r="CG5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="CH5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="CJ5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="CK5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="CM5" s="22"/>
+      <c r="CN5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="CO5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="CQ5" s="22"/>
+      <c r="CR5" s="22"/>
+      <c r="CS5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="CT5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="CV5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="CW5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="CY5" s="22"/>
+      <c r="CZ5" s="22"/>
+    </row>
+    <row r="6" spans="2:105" ht="34.5" customHeight="1">
       <c r="B6" s="25" t="s">
         <v>478</v>
       </c>
@@ -11571,20 +11753,81 @@
       <c r="BH6" s="25" t="s">
         <v>934</v>
       </c>
-      <c r="BJ6" s="25" t="s">
+      <c r="BI6" s="35"/>
+      <c r="BJ6" s="36" t="s">
         <v>781</v>
       </c>
-      <c r="BK6" s="25" t="s">
+      <c r="BK6" s="36" t="s">
         <v>782</v>
       </c>
-      <c r="BM6" s="25" t="s">
+      <c r="BL6" s="35"/>
+      <c r="BM6" s="36" t="s">
         <v>264</v>
       </c>
-      <c r="BN6" s="25" t="s">
+      <c r="BN6" s="36" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="7" spans="2:67" ht="18.75" customHeight="1">
+      <c r="BO6" s="35"/>
+      <c r="BP6" s="35"/>
+      <c r="BQ6" s="35"/>
+      <c r="BR6" s="36" t="s">
+        <v>633</v>
+      </c>
+      <c r="BS6" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="BT6" s="35"/>
+      <c r="BU6" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="BV6" s="36" t="s">
+        <v>657</v>
+      </c>
+      <c r="BW6" s="35"/>
+      <c r="BX6" s="36" t="s">
+        <v>349</v>
+      </c>
+      <c r="BY6" s="36" t="s">
+        <v>350</v>
+      </c>
+      <c r="CB6" s="25" t="s">
+        <v>468</v>
+      </c>
+      <c r="CC6" s="25" t="s">
+        <v>469</v>
+      </c>
+      <c r="CG6" s="25" t="s">
+        <v>203</v>
+      </c>
+      <c r="CH6" s="25" t="s">
+        <v>204</v>
+      </c>
+      <c r="CJ6" s="25" t="s">
+        <v>207</v>
+      </c>
+      <c r="CK6" s="25" t="s">
+        <v>208</v>
+      </c>
+      <c r="CN6" s="25" t="s">
+        <v>403</v>
+      </c>
+      <c r="CO6" s="25" t="s">
+        <v>404</v>
+      </c>
+      <c r="CS6" s="25" t="s">
+        <v>251</v>
+      </c>
+      <c r="CT6" s="25" t="s">
+        <v>252</v>
+      </c>
+      <c r="CV6" s="25" t="s">
+        <v>253</v>
+      </c>
+      <c r="CW6" s="25" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="7" spans="2:105" ht="18.75" customHeight="1">
       <c r="B7" s="25" t="s">
         <v>488</v>
       </c>
@@ -11689,20 +11932,81 @@
       <c r="BH7" s="25" t="s">
         <v>935</v>
       </c>
-      <c r="BJ7" s="25" t="s">
+      <c r="BI7" s="35"/>
+      <c r="BJ7" s="36" t="s">
         <v>783</v>
       </c>
-      <c r="BK7" s="25" t="s">
+      <c r="BK7" s="36" t="s">
         <v>784</v>
       </c>
-      <c r="BM7" s="25" t="s">
+      <c r="BL7" s="35"/>
+      <c r="BM7" s="36" t="s">
         <v>266</v>
       </c>
-      <c r="BN7" s="25" t="s">
+      <c r="BN7" s="36" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="8" spans="2:67" ht="18.75" customHeight="1">
+      <c r="BO7" s="35"/>
+      <c r="BP7" s="35"/>
+      <c r="BQ7" s="35"/>
+      <c r="BR7" s="36" t="s">
+        <v>118</v>
+      </c>
+      <c r="BS7" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="BT7" s="35"/>
+      <c r="BU7" s="36" t="s">
+        <v>64</v>
+      </c>
+      <c r="BV7" s="36" t="s">
+        <v>658</v>
+      </c>
+      <c r="BW7" s="35"/>
+      <c r="BX7" s="36" t="s">
+        <v>351</v>
+      </c>
+      <c r="BY7" s="36" t="s">
+        <v>352</v>
+      </c>
+      <c r="CB7" s="25" t="s">
+        <v>470</v>
+      </c>
+      <c r="CC7" s="25" t="s">
+        <v>471</v>
+      </c>
+      <c r="CG7" s="25" t="s">
+        <v>205</v>
+      </c>
+      <c r="CH7" s="25" t="s">
+        <v>206</v>
+      </c>
+      <c r="CJ7" s="25" t="s">
+        <v>209</v>
+      </c>
+      <c r="CK7" s="25" t="s">
+        <v>210</v>
+      </c>
+      <c r="CN7" s="25" t="s">
+        <v>405</v>
+      </c>
+      <c r="CO7" s="25" t="s">
+        <v>406</v>
+      </c>
+      <c r="CS7" s="25" t="s">
+        <v>323</v>
+      </c>
+      <c r="CT7" s="25" t="s">
+        <v>324</v>
+      </c>
+      <c r="CV7" s="25" t="s">
+        <v>255</v>
+      </c>
+      <c r="CW7" s="25" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="2:105" ht="18.75" customHeight="1">
       <c r="B8" s="25" t="s">
         <v>539</v>
       </c>
@@ -11810,20 +12114,59 @@
       <c r="BH8" s="25" t="s">
         <v>936</v>
       </c>
-      <c r="BJ8" s="25" t="s">
+      <c r="BI8" s="35"/>
+      <c r="BJ8" s="36" t="s">
         <v>785</v>
       </c>
-      <c r="BK8" s="25" t="s">
+      <c r="BK8" s="36" t="s">
         <v>786</v>
       </c>
-      <c r="BM8" s="25" t="s">
+      <c r="BL8" s="35"/>
+      <c r="BM8" s="36" t="s">
         <v>272</v>
       </c>
-      <c r="BN8" s="25" t="s">
+      <c r="BN8" s="36" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="9" spans="2:67" ht="20.25" customHeight="1">
+      <c r="BO8" s="35"/>
+      <c r="BP8" s="35"/>
+      <c r="BQ8" s="35"/>
+      <c r="BR8" s="36" t="s">
+        <v>98</v>
+      </c>
+      <c r="BS8" s="36" t="s">
+        <v>634</v>
+      </c>
+      <c r="BT8" s="35"/>
+      <c r="BU8" s="35"/>
+      <c r="BV8" s="35"/>
+      <c r="BW8" s="35"/>
+      <c r="BX8" s="36" t="s">
+        <v>353</v>
+      </c>
+      <c r="BY8" s="36" t="s">
+        <v>354</v>
+      </c>
+      <c r="CB8" s="25" t="s">
+        <v>110</v>
+      </c>
+      <c r="CC8" s="25" t="s">
+        <v>192</v>
+      </c>
+      <c r="CJ8" s="25" t="s">
+        <v>211</v>
+      </c>
+      <c r="CK8" s="25" t="s">
+        <v>212</v>
+      </c>
+      <c r="CN8" s="25" t="s">
+        <v>407</v>
+      </c>
+      <c r="CO8" s="25" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="9" spans="2:105" ht="20.25" customHeight="1">
       <c r="B9" s="25" t="s">
         <v>541</v>
       </c>
@@ -11930,20 +12273,59 @@
       <c r="BH9" s="25" t="s">
         <v>937</v>
       </c>
-      <c r="BJ9" s="25" t="s">
+      <c r="BI9" s="35"/>
+      <c r="BJ9" s="36" t="s">
         <v>785</v>
       </c>
-      <c r="BK9" s="25" t="s">
+      <c r="BK9" s="36" t="s">
         <v>787</v>
       </c>
-      <c r="BM9" s="25" t="s">
+      <c r="BL9" s="35"/>
+      <c r="BM9" s="36" t="s">
         <v>274</v>
       </c>
-      <c r="BN9" s="25" t="s">
+      <c r="BN9" s="36" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="10" spans="2:67" ht="30">
+      <c r="BO9" s="35"/>
+      <c r="BP9" s="35"/>
+      <c r="BQ9" s="35"/>
+      <c r="BR9" s="36" t="s">
+        <v>81</v>
+      </c>
+      <c r="BS9" s="36" t="s">
+        <v>635</v>
+      </c>
+      <c r="BT9" s="35"/>
+      <c r="BU9" s="35"/>
+      <c r="BV9" s="35"/>
+      <c r="BW9" s="35"/>
+      <c r="BX9" s="36" t="s">
+        <v>355</v>
+      </c>
+      <c r="BY9" s="36" t="s">
+        <v>356</v>
+      </c>
+      <c r="CB9" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="CC9" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="CJ9" s="25" t="s">
+        <v>213</v>
+      </c>
+      <c r="CK9" s="25" t="s">
+        <v>214</v>
+      </c>
+      <c r="CN9" s="25" t="s">
+        <v>409</v>
+      </c>
+      <c r="CO9" s="25" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="10" spans="2:105" ht="31.5">
       <c r="B10" s="25" t="s">
         <v>543</v>
       </c>
@@ -12040,20 +12422,59 @@
       <c r="BH10" s="25" t="s">
         <v>938</v>
       </c>
-      <c r="BJ10" s="25" t="s">
+      <c r="BI10" s="35"/>
+      <c r="BJ10" s="36" t="s">
         <v>788</v>
       </c>
-      <c r="BK10" s="25" t="s">
+      <c r="BK10" s="36" t="s">
         <v>789</v>
       </c>
-      <c r="BM10" s="25" t="s">
+      <c r="BL10" s="35"/>
+      <c r="BM10" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="BN10" s="25" t="s">
+      <c r="BN10" s="36" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="11" spans="2:67" ht="20.25" customHeight="1">
+      <c r="BO10" s="35"/>
+      <c r="BP10" s="35"/>
+      <c r="BQ10" s="35"/>
+      <c r="BR10" s="36" t="s">
+        <v>62</v>
+      </c>
+      <c r="BS10" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="BT10" s="35"/>
+      <c r="BU10" s="35"/>
+      <c r="BV10" s="35"/>
+      <c r="BW10" s="35"/>
+      <c r="BX10" s="36" t="s">
+        <v>357</v>
+      </c>
+      <c r="BY10" s="36" t="s">
+        <v>358</v>
+      </c>
+      <c r="CB10" s="25" t="s">
+        <v>199</v>
+      </c>
+      <c r="CC10" s="25" t="s">
+        <v>200</v>
+      </c>
+      <c r="CJ10" s="25" t="s">
+        <v>215</v>
+      </c>
+      <c r="CK10" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="CN10" s="25" t="s">
+        <v>411</v>
+      </c>
+      <c r="CO10" s="25" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="11" spans="2:105" ht="20.25" customHeight="1">
       <c r="B11" s="25" t="s">
         <v>547</v>
       </c>
@@ -12150,20 +12571,59 @@
       <c r="BH11" s="25" t="s">
         <v>939</v>
       </c>
-      <c r="BJ11" s="25" t="s">
+      <c r="BI11" s="35"/>
+      <c r="BJ11" s="36" t="s">
         <v>788</v>
       </c>
-      <c r="BK11" s="25" t="s">
+      <c r="BK11" s="36" t="s">
         <v>790</v>
       </c>
-      <c r="BM11" s="25" t="s">
+      <c r="BL11" s="35"/>
+      <c r="BM11" s="36" t="s">
         <v>279</v>
       </c>
-      <c r="BN11" s="25" t="s">
+      <c r="BN11" s="36" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="12" spans="2:67" ht="18" customHeight="1">
+      <c r="BO11" s="35"/>
+      <c r="BP11" s="35"/>
+      <c r="BQ11" s="35"/>
+      <c r="BR11" s="36" t="s">
+        <v>80</v>
+      </c>
+      <c r="BS11" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="BT11" s="35"/>
+      <c r="BU11" s="35"/>
+      <c r="BV11" s="35"/>
+      <c r="BW11" s="35"/>
+      <c r="BX11" s="36" t="s">
+        <v>359</v>
+      </c>
+      <c r="BY11" s="36" t="s">
+        <v>360</v>
+      </c>
+      <c r="CB11" s="25" t="s">
+        <v>201</v>
+      </c>
+      <c r="CC11" s="25" t="s">
+        <v>202</v>
+      </c>
+      <c r="CJ11" s="25" t="s">
+        <v>217</v>
+      </c>
+      <c r="CK11" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="CN11" s="25" t="s">
+        <v>413</v>
+      </c>
+      <c r="CO11" s="25" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="12" spans="2:105" ht="18" customHeight="1">
       <c r="B12" s="25" t="s">
         <v>549</v>
       </c>
@@ -12260,20 +12720,53 @@
       <c r="BH12" s="25" t="s">
         <v>940</v>
       </c>
-      <c r="BJ12" s="25" t="s">
+      <c r="BI12" s="35"/>
+      <c r="BJ12" s="36" t="s">
         <v>791</v>
       </c>
-      <c r="BK12" s="25" t="s">
+      <c r="BK12" s="36" t="s">
         <v>792</v>
       </c>
-      <c r="BM12" s="25" t="s">
+      <c r="BL12" s="35"/>
+      <c r="BM12" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="BN12" s="25" t="s">
+      <c r="BN12" s="36" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="13" spans="2:67" ht="30">
+      <c r="BO12" s="35"/>
+      <c r="BP12" s="35"/>
+      <c r="BQ12" s="35"/>
+      <c r="BR12" s="36" t="s">
+        <v>636</v>
+      </c>
+      <c r="BS12" s="36" t="s">
+        <v>637</v>
+      </c>
+      <c r="BT12" s="35"/>
+      <c r="BU12" s="35"/>
+      <c r="BV12" s="35"/>
+      <c r="BW12" s="35"/>
+      <c r="BX12" s="36" t="s">
+        <v>361</v>
+      </c>
+      <c r="BY12" s="36" t="s">
+        <v>362</v>
+      </c>
+      <c r="CJ12" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="CK12" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="CN12" s="25" t="s">
+        <v>415</v>
+      </c>
+      <c r="CO12" s="25" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="13" spans="2:105" ht="31.5">
       <c r="B13" s="25" t="s">
         <v>553</v>
       </c>
@@ -12364,20 +12857,53 @@
       <c r="BH13" s="25" t="s">
         <v>941</v>
       </c>
-      <c r="BJ13" s="25" t="s">
+      <c r="BI13" s="35"/>
+      <c r="BJ13" s="36" t="s">
         <v>793</v>
       </c>
-      <c r="BK13" s="25" t="s">
+      <c r="BK13" s="36" t="s">
         <v>794</v>
       </c>
-      <c r="BM13" s="25" t="s">
+      <c r="BL13" s="35"/>
+      <c r="BM13" s="36" t="s">
         <v>284</v>
       </c>
-      <c r="BN13" s="25" t="s">
+      <c r="BN13" s="36" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="14" spans="2:67" ht="30">
+      <c r="BO13" s="35"/>
+      <c r="BP13" s="35"/>
+      <c r="BQ13" s="35"/>
+      <c r="BR13" s="36" t="s">
+        <v>117</v>
+      </c>
+      <c r="BS13" s="36" t="s">
+        <v>638</v>
+      </c>
+      <c r="BT13" s="35"/>
+      <c r="BU13" s="35"/>
+      <c r="BV13" s="35"/>
+      <c r="BW13" s="35"/>
+      <c r="BX13" s="36" t="s">
+        <v>363</v>
+      </c>
+      <c r="BY13" s="36" t="s">
+        <v>364</v>
+      </c>
+      <c r="CJ13" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="CK13" s="25" t="s">
+        <v>222</v>
+      </c>
+      <c r="CN13" s="25" t="s">
+        <v>417</v>
+      </c>
+      <c r="CO13" s="25" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="14" spans="2:105" ht="31.5">
       <c r="E14" s="25" t="s">
         <v>520</v>
       </c>
@@ -12462,20 +12988,55 @@
       <c r="BH14" s="25" t="s">
         <v>942</v>
       </c>
-      <c r="BJ14" s="25" t="s">
+      <c r="BI14" s="35"/>
+      <c r="BJ14" s="36" t="s">
         <v>793</v>
       </c>
-      <c r="BK14" s="25" t="s">
+      <c r="BK14" s="36" t="s">
         <v>795</v>
       </c>
-      <c r="BM14" s="25" t="s">
+      <c r="BL14" s="35"/>
+      <c r="BM14" s="36" t="s">
         <v>286</v>
       </c>
-      <c r="BN14" s="25" t="s">
+      <c r="BN14" s="36" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="15" spans="2:67" ht="45">
+      <c r="BO14" s="35"/>
+      <c r="BP14" s="35"/>
+      <c r="BQ14" s="35"/>
+      <c r="BR14" s="36" t="s">
+        <v>97</v>
+      </c>
+      <c r="BS14" s="36" t="s">
+        <v>639</v>
+      </c>
+      <c r="BT14" s="35"/>
+      <c r="BU14" s="35"/>
+      <c r="BV14" s="35"/>
+      <c r="BW14" s="35"/>
+      <c r="BX14" s="36" t="s">
+        <v>365</v>
+      </c>
+      <c r="BY14" s="36" t="s">
+        <v>366</v>
+      </c>
+      <c r="CJ14" s="25" t="s">
+        <v>223</v>
+      </c>
+      <c r="CK14" s="25" t="s">
+        <v>224</v>
+      </c>
+      <c r="CN14" s="25" t="s">
+        <v>419</v>
+      </c>
+      <c r="CO14" s="25" t="s">
+        <v>420</v>
+      </c>
+      <c r="CZ14" s="34"/>
+      <c r="DA14" s="34"/>
+    </row>
+    <row r="15" spans="2:105" ht="45">
       <c r="E15" s="25" t="s">
         <v>522</v>
       </c>
@@ -12552,20 +13113,55 @@
       <c r="BH15" s="25" t="s">
         <v>943</v>
       </c>
-      <c r="BJ15" s="25" t="s">
+      <c r="BI15" s="35"/>
+      <c r="BJ15" s="36" t="s">
         <v>793</v>
       </c>
-      <c r="BK15" s="25" t="s">
+      <c r="BK15" s="36" t="s">
         <v>796</v>
       </c>
-      <c r="BM15" s="25" t="s">
+      <c r="BL15" s="35"/>
+      <c r="BM15" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="BN15" s="25" t="s">
+      <c r="BN15" s="36" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="16" spans="2:67" ht="30">
+      <c r="BO15" s="35"/>
+      <c r="BP15" s="35"/>
+      <c r="BQ15" s="35"/>
+      <c r="BR15" s="36" t="s">
+        <v>79</v>
+      </c>
+      <c r="BS15" s="36" t="s">
+        <v>640</v>
+      </c>
+      <c r="BT15" s="35"/>
+      <c r="BU15" s="35"/>
+      <c r="BV15" s="35"/>
+      <c r="BW15" s="35"/>
+      <c r="BX15" s="36" t="s">
+        <v>367</v>
+      </c>
+      <c r="BY15" s="36" t="s">
+        <v>368</v>
+      </c>
+      <c r="CJ15" s="25" t="s">
+        <v>225</v>
+      </c>
+      <c r="CK15" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="CN15" s="25" t="s">
+        <v>421</v>
+      </c>
+      <c r="CO15" s="25" t="s">
+        <v>422</v>
+      </c>
+      <c r="CZ15" s="34"/>
+      <c r="DA15" s="34"/>
+    </row>
+    <row r="16" spans="2:105" ht="31.5">
       <c r="E16" s="25" t="s">
         <v>524</v>
       </c>
@@ -12638,20 +13234,55 @@
       <c r="BH16" s="25" t="s">
         <v>944</v>
       </c>
-      <c r="BJ16" s="25" t="s">
+      <c r="BI16" s="35"/>
+      <c r="BJ16" s="36" t="s">
         <v>793</v>
       </c>
-      <c r="BK16" s="25" t="s">
+      <c r="BK16" s="36" t="s">
         <v>797</v>
       </c>
-      <c r="BM16" s="25" t="s">
+      <c r="BL16" s="35"/>
+      <c r="BM16" s="36" t="s">
         <v>289</v>
       </c>
-      <c r="BN16" s="25" t="s">
+      <c r="BN16" s="36" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="17" spans="5:66" ht="30">
+      <c r="BO16" s="35"/>
+      <c r="BP16" s="35"/>
+      <c r="BQ16" s="35"/>
+      <c r="BR16" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="BS16" s="36" t="s">
+        <v>641</v>
+      </c>
+      <c r="BT16" s="35"/>
+      <c r="BU16" s="35"/>
+      <c r="BV16" s="35"/>
+      <c r="BW16" s="35"/>
+      <c r="BX16" s="36" t="s">
+        <v>369</v>
+      </c>
+      <c r="BY16" s="36" t="s">
+        <v>370</v>
+      </c>
+      <c r="CJ16" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="CK16" s="25" t="s">
+        <v>228</v>
+      </c>
+      <c r="CN16" s="25" t="s">
+        <v>423</v>
+      </c>
+      <c r="CO16" s="25" t="s">
+        <v>424</v>
+      </c>
+      <c r="CZ16" s="34"/>
+      <c r="DA16" s="34"/>
+    </row>
+    <row r="17" spans="5:105" ht="31.5">
       <c r="E17" s="25" t="s">
         <v>526</v>
       </c>
@@ -12724,20 +13355,55 @@
       <c r="BH17" s="25" t="s">
         <v>945</v>
       </c>
-      <c r="BJ17" s="25" t="s">
+      <c r="BI17" s="35"/>
+      <c r="BJ17" s="36" t="s">
         <v>798</v>
       </c>
-      <c r="BK17" s="25" t="s">
+      <c r="BK17" s="36" t="s">
         <v>799</v>
       </c>
-      <c r="BM17" s="25" t="s">
+      <c r="BL17" s="35"/>
+      <c r="BM17" s="36" t="s">
         <v>291</v>
       </c>
-      <c r="BN17" s="25" t="s">
+      <c r="BN17" s="36" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="18" spans="5:66" ht="30">
+      <c r="BO17" s="35"/>
+      <c r="BP17" s="35"/>
+      <c r="BQ17" s="35"/>
+      <c r="BR17" s="36" t="s">
+        <v>78</v>
+      </c>
+      <c r="BS17" s="36" t="s">
+        <v>642</v>
+      </c>
+      <c r="BT17" s="35"/>
+      <c r="BU17" s="35"/>
+      <c r="BV17" s="35"/>
+      <c r="BW17" s="35"/>
+      <c r="BX17" s="36" t="s">
+        <v>371</v>
+      </c>
+      <c r="BY17" s="36" t="s">
+        <v>372</v>
+      </c>
+      <c r="CJ17" s="25" t="s">
+        <v>229</v>
+      </c>
+      <c r="CK17" s="25" t="s">
+        <v>230</v>
+      </c>
+      <c r="CN17" s="25" t="s">
+        <v>425</v>
+      </c>
+      <c r="CO17" s="25" t="s">
+        <v>426</v>
+      </c>
+      <c r="CZ17" s="34"/>
+      <c r="DA17" s="34"/>
+    </row>
+    <row r="18" spans="5:105" ht="31.5">
       <c r="E18" s="25" t="s">
         <v>529</v>
       </c>
@@ -12800,20 +13466,51 @@
       <c r="BH18" s="25" t="s">
         <v>946</v>
       </c>
-      <c r="BJ18" s="25" t="s">
+      <c r="BI18" s="35"/>
+      <c r="BJ18" s="36" t="s">
         <v>800</v>
       </c>
-      <c r="BK18" s="25" t="s">
+      <c r="BK18" s="36" t="s">
         <v>801</v>
       </c>
-      <c r="BM18" s="25" t="s">
+      <c r="BL18" s="35"/>
+      <c r="BM18" s="36" t="s">
         <v>293</v>
       </c>
-      <c r="BN18" s="25" t="s">
+      <c r="BN18" s="36" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="19" spans="5:66" ht="30">
+      <c r="BO18" s="35"/>
+      <c r="BP18" s="35"/>
+      <c r="BQ18" s="35"/>
+      <c r="BR18" s="36" t="s">
+        <v>643</v>
+      </c>
+      <c r="BS18" s="36" t="s">
+        <v>644</v>
+      </c>
+      <c r="BT18" s="35"/>
+      <c r="BU18" s="35"/>
+      <c r="BV18" s="35"/>
+      <c r="BW18" s="35"/>
+      <c r="BX18" s="35"/>
+      <c r="BY18" s="35"/>
+      <c r="CJ18" s="25" t="s">
+        <v>231</v>
+      </c>
+      <c r="CK18" s="25" t="s">
+        <v>232</v>
+      </c>
+      <c r="CN18" s="25" t="s">
+        <v>378</v>
+      </c>
+      <c r="CO18" s="25" t="s">
+        <v>379</v>
+      </c>
+      <c r="CZ18" s="34"/>
+      <c r="DA18" s="34"/>
+    </row>
+    <row r="19" spans="5:105" ht="30">
       <c r="E19" s="25" t="s">
         <v>531</v>
       </c>
@@ -12876,20 +13573,51 @@
       <c r="BH19" s="25" t="s">
         <v>947</v>
       </c>
-      <c r="BJ19" s="25" t="s">
+      <c r="BI19" s="35"/>
+      <c r="BJ19" s="36" t="s">
         <v>802</v>
       </c>
-      <c r="BK19" s="25" t="s">
+      <c r="BK19" s="36" t="s">
         <v>803</v>
       </c>
-      <c r="BM19" s="25" t="s">
+      <c r="BL19" s="35"/>
+      <c r="BM19" s="36" t="s">
         <v>295</v>
       </c>
-      <c r="BN19" s="25" t="s">
+      <c r="BN19" s="36" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="20" spans="5:66" ht="30">
+      <c r="BO19" s="35"/>
+      <c r="BP19" s="35"/>
+      <c r="BQ19" s="35"/>
+      <c r="BR19" s="36" t="s">
+        <v>116</v>
+      </c>
+      <c r="BS19" s="36" t="s">
+        <v>645</v>
+      </c>
+      <c r="BT19" s="35"/>
+      <c r="BU19" s="35"/>
+      <c r="BV19" s="35"/>
+      <c r="BW19" s="35"/>
+      <c r="BX19" s="35"/>
+      <c r="BY19" s="35"/>
+      <c r="CJ19" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="CK19" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="CN19" s="25" t="s">
+        <v>380</v>
+      </c>
+      <c r="CO19" s="25" t="s">
+        <v>381</v>
+      </c>
+      <c r="CZ19" s="34"/>
+      <c r="DA19" s="34"/>
+    </row>
+    <row r="20" spans="5:105" ht="31.5">
       <c r="E20" s="25" t="s">
         <v>533</v>
       </c>
@@ -12952,14 +13680,47 @@
       <c r="BH20" s="25" t="s">
         <v>948</v>
       </c>
-      <c r="BJ20" s="25" t="s">
+      <c r="BI20" s="35"/>
+      <c r="BJ20" s="36" t="s">
         <v>804</v>
       </c>
-      <c r="BK20" s="25" t="s">
+      <c r="BK20" s="36" t="s">
         <v>805</v>
       </c>
-    </row>
-    <row r="21" spans="5:66" ht="30">
+      <c r="BL20" s="35"/>
+      <c r="BM20" s="35"/>
+      <c r="BN20" s="35"/>
+      <c r="BO20" s="35"/>
+      <c r="BP20" s="35"/>
+      <c r="BQ20" s="35"/>
+      <c r="BR20" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="BS20" s="36" t="s">
+        <v>646</v>
+      </c>
+      <c r="BT20" s="35"/>
+      <c r="BU20" s="35"/>
+      <c r="BV20" s="35"/>
+      <c r="BW20" s="35"/>
+      <c r="BX20" s="35"/>
+      <c r="BY20" s="35"/>
+      <c r="CJ20" s="25" t="s">
+        <v>235</v>
+      </c>
+      <c r="CK20" s="25" t="s">
+        <v>86</v>
+      </c>
+      <c r="CN20" s="25" t="s">
+        <v>382</v>
+      </c>
+      <c r="CO20" s="25" t="s">
+        <v>383</v>
+      </c>
+      <c r="CZ20" s="34"/>
+      <c r="DA20" s="34"/>
+    </row>
+    <row r="21" spans="5:105" ht="31.5">
       <c r="O21" s="25" t="s">
         <v>34</v>
       </c>
@@ -13008,14 +13769,45 @@
       <c r="BH21" s="25" t="s">
         <v>949</v>
       </c>
-      <c r="BJ21" s="25" t="s">
+      <c r="BI21" s="35"/>
+      <c r="BJ21" s="36" t="s">
         <v>804</v>
       </c>
-      <c r="BK21" s="25" t="s">
+      <c r="BK21" s="36" t="s">
         <v>806</v>
       </c>
-    </row>
-    <row r="22" spans="5:66" ht="30">
+      <c r="BL21" s="35"/>
+      <c r="BM21" s="35"/>
+      <c r="BN21" s="35"/>
+      <c r="BO21" s="35"/>
+      <c r="BP21" s="35"/>
+      <c r="BQ21" s="35"/>
+      <c r="BR21" s="36" t="s">
+        <v>77</v>
+      </c>
+      <c r="BS21" s="36" t="s">
+        <v>647</v>
+      </c>
+      <c r="BT21" s="35"/>
+      <c r="BU21" s="35"/>
+      <c r="BV21" s="35"/>
+      <c r="BW21" s="35"/>
+      <c r="BX21" s="35"/>
+      <c r="BY21" s="35"/>
+      <c r="CJ21" s="25" t="s">
+        <v>236</v>
+      </c>
+      <c r="CK21" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="CN21" s="25" t="s">
+        <v>384</v>
+      </c>
+      <c r="CO21" s="25" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="22" spans="5:105" ht="31.5">
       <c r="O22" s="25" t="s">
         <v>103</v>
       </c>
@@ -13058,14 +13850,39 @@
       <c r="BH22" s="25" t="s">
         <v>950</v>
       </c>
-      <c r="BJ22" s="25" t="s">
+      <c r="BI22" s="35"/>
+      <c r="BJ22" s="36" t="s">
         <v>807</v>
       </c>
-      <c r="BK22" s="25" t="s">
+      <c r="BK22" s="36" t="s">
         <v>808</v>
       </c>
-    </row>
-    <row r="23" spans="5:66" ht="30.75" thickBot="1">
+      <c r="BL22" s="35"/>
+      <c r="BM22" s="35"/>
+      <c r="BN22" s="35"/>
+      <c r="BO22" s="35"/>
+      <c r="BP22" s="35"/>
+      <c r="BQ22" s="35"/>
+      <c r="BR22" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="BS22" s="36" t="s">
+        <v>648</v>
+      </c>
+      <c r="BT22" s="35"/>
+      <c r="BU22" s="35"/>
+      <c r="BV22" s="35"/>
+      <c r="BW22" s="35"/>
+      <c r="BX22" s="35"/>
+      <c r="BY22" s="35"/>
+      <c r="CN22" s="25" t="s">
+        <v>386</v>
+      </c>
+      <c r="CO22" s="25" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="23" spans="5:105" ht="45.75" thickBot="1">
       <c r="O23" s="25" t="s">
         <v>154</v>
       </c>
@@ -13108,14 +13925,39 @@
       <c r="BH23" s="25" t="s">
         <v>951</v>
       </c>
-      <c r="BJ23" s="25" t="s">
+      <c r="BI23" s="35"/>
+      <c r="BJ23" s="36" t="s">
         <v>807</v>
       </c>
-      <c r="BK23" s="25" t="s">
+      <c r="BK23" s="36" t="s">
         <v>809</v>
       </c>
-    </row>
-    <row r="24" spans="5:66" ht="30.75" thickBot="1">
+      <c r="BL23" s="35"/>
+      <c r="BM23" s="35"/>
+      <c r="BN23" s="35"/>
+      <c r="BO23" s="35"/>
+      <c r="BP23" s="35"/>
+      <c r="BQ23" s="35"/>
+      <c r="BR23" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="BS23" s="36" t="s">
+        <v>649</v>
+      </c>
+      <c r="BT23" s="35"/>
+      <c r="BU23" s="35"/>
+      <c r="BV23" s="35"/>
+      <c r="BW23" s="35"/>
+      <c r="BX23" s="35"/>
+      <c r="BY23" s="35"/>
+      <c r="CN23" s="25" t="s">
+        <v>388</v>
+      </c>
+      <c r="CO23" s="25" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="24" spans="5:105" ht="30.75" thickBot="1">
       <c r="O24" s="25" t="s">
         <v>156</v>
       </c>
@@ -13158,14 +14000,39 @@
       <c r="BH24" s="25" t="s">
         <v>952</v>
       </c>
-      <c r="BJ24" s="25" t="s">
+      <c r="BI24" s="35"/>
+      <c r="BJ24" s="36" t="s">
         <v>810</v>
       </c>
-      <c r="BK24" s="25" t="s">
+      <c r="BK24" s="36" t="s">
         <v>811</v>
       </c>
-    </row>
-    <row r="25" spans="5:66" ht="30">
+      <c r="BL24" s="35"/>
+      <c r="BM24" s="35"/>
+      <c r="BN24" s="35"/>
+      <c r="BO24" s="35"/>
+      <c r="BP24" s="35"/>
+      <c r="BQ24" s="35"/>
+      <c r="BR24" s="36" t="s">
+        <v>650</v>
+      </c>
+      <c r="BS24" s="36" t="s">
+        <v>651</v>
+      </c>
+      <c r="BT24" s="35"/>
+      <c r="BU24" s="35"/>
+      <c r="BV24" s="35"/>
+      <c r="BW24" s="35"/>
+      <c r="BX24" s="35"/>
+      <c r="BY24" s="35"/>
+      <c r="CN24" s="25" t="s">
+        <v>390</v>
+      </c>
+      <c r="CO24" s="25" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="25" spans="5:105" ht="31.5">
       <c r="O25" s="25" t="s">
         <v>158</v>
       </c>
@@ -13202,14 +14069,39 @@
       <c r="BH25" s="25" t="s">
         <v>953</v>
       </c>
-      <c r="BJ25" s="25" t="s">
+      <c r="BI25" s="35"/>
+      <c r="BJ25" s="36" t="s">
         <v>812</v>
       </c>
-      <c r="BK25" s="25" t="s">
+      <c r="BK25" s="36" t="s">
         <v>813</v>
       </c>
-    </row>
-    <row r="26" spans="5:66" ht="30">
+      <c r="BL25" s="35"/>
+      <c r="BM25" s="35"/>
+      <c r="BN25" s="35"/>
+      <c r="BO25" s="35"/>
+      <c r="BP25" s="35"/>
+      <c r="BQ25" s="35"/>
+      <c r="BR25" s="36" t="s">
+        <v>115</v>
+      </c>
+      <c r="BS25" s="36" t="s">
+        <v>652</v>
+      </c>
+      <c r="BT25" s="35"/>
+      <c r="BU25" s="35"/>
+      <c r="BV25" s="35"/>
+      <c r="BW25" s="35"/>
+      <c r="BX25" s="35"/>
+      <c r="BY25" s="35"/>
+      <c r="CN25" s="25" t="s">
+        <v>392</v>
+      </c>
+      <c r="CO25" s="25" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="26" spans="5:105" ht="31.5">
       <c r="O26" s="25" t="s">
         <v>160</v>
       </c>
@@ -13246,14 +14138,39 @@
       <c r="BH26" s="25" t="s">
         <v>954</v>
       </c>
-      <c r="BJ26" s="25" t="s">
+      <c r="BI26" s="35"/>
+      <c r="BJ26" s="36" t="s">
         <v>814</v>
       </c>
-      <c r="BK26" s="25" t="s">
+      <c r="BK26" s="36" t="s">
         <v>815</v>
       </c>
-    </row>
-    <row r="27" spans="5:66" ht="30">
+      <c r="BL26" s="35"/>
+      <c r="BM26" s="35"/>
+      <c r="BN26" s="35"/>
+      <c r="BO26" s="35"/>
+      <c r="BP26" s="35"/>
+      <c r="BQ26" s="35"/>
+      <c r="BR26" s="36" t="s">
+        <v>75</v>
+      </c>
+      <c r="BS26" s="36" t="s">
+        <v>653</v>
+      </c>
+      <c r="BT26" s="35"/>
+      <c r="BU26" s="35"/>
+      <c r="BV26" s="35"/>
+      <c r="BW26" s="35"/>
+      <c r="BX26" s="35"/>
+      <c r="BY26" s="35"/>
+      <c r="CN26" s="25" t="s">
+        <v>394</v>
+      </c>
+      <c r="CO26" s="25" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="27" spans="5:105" ht="31.5">
       <c r="O27" s="25" t="s">
         <v>35</v>
       </c>
@@ -13290,14 +14207,39 @@
       <c r="BH27" s="25" t="s">
         <v>955</v>
       </c>
-      <c r="BJ27" s="25" t="s">
+      <c r="BI27" s="35"/>
+      <c r="BJ27" s="36" t="s">
         <v>814</v>
       </c>
-      <c r="BK27" s="25" t="s">
+      <c r="BK27" s="36" t="s">
         <v>816</v>
       </c>
-    </row>
-    <row r="28" spans="5:66" ht="30">
+      <c r="BL27" s="35"/>
+      <c r="BM27" s="35"/>
+      <c r="BN27" s="35"/>
+      <c r="BO27" s="35"/>
+      <c r="BP27" s="35"/>
+      <c r="BQ27" s="35"/>
+      <c r="BR27" s="36" t="s">
+        <v>95</v>
+      </c>
+      <c r="BS27" s="36" t="s">
+        <v>654</v>
+      </c>
+      <c r="BT27" s="35"/>
+      <c r="BU27" s="35"/>
+      <c r="BV27" s="35"/>
+      <c r="BW27" s="35"/>
+      <c r="BX27" s="35"/>
+      <c r="BY27" s="35"/>
+      <c r="CN27" s="25" t="s">
+        <v>396</v>
+      </c>
+      <c r="CO27" s="25" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="28" spans="5:105" ht="31.5">
       <c r="O28" s="25" t="s">
         <v>163</v>
       </c>
@@ -13334,14 +14276,39 @@
       <c r="BH28" s="25" t="s">
         <v>956</v>
       </c>
-      <c r="BJ28" s="25" t="s">
+      <c r="BI28" s="35"/>
+      <c r="BJ28" s="36" t="s">
         <v>817</v>
       </c>
-      <c r="BK28" s="25" t="s">
+      <c r="BK28" s="36" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="29" spans="5:66" ht="30">
+      <c r="BL28" s="35"/>
+      <c r="BM28" s="35"/>
+      <c r="BN28" s="35"/>
+      <c r="BO28" s="35"/>
+      <c r="BP28" s="35"/>
+      <c r="BQ28" s="35"/>
+      <c r="BR28" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="BS28" s="36" t="s">
+        <v>655</v>
+      </c>
+      <c r="BT28" s="35"/>
+      <c r="BU28" s="35"/>
+      <c r="BV28" s="35"/>
+      <c r="BW28" s="35"/>
+      <c r="BX28" s="35"/>
+      <c r="BY28" s="35"/>
+      <c r="CN28" s="25" t="s">
+        <v>398</v>
+      </c>
+      <c r="CO28" s="25" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="29" spans="5:105" ht="31.5">
       <c r="O29" s="25" t="s">
         <v>105</v>
       </c>
@@ -13378,14 +14345,39 @@
       <c r="BH29" s="25" t="s">
         <v>957</v>
       </c>
-      <c r="BJ29" s="25" t="s">
+      <c r="BI29" s="35"/>
+      <c r="BJ29" s="36" t="s">
         <v>817</v>
       </c>
-      <c r="BK29" s="25" t="s">
+      <c r="BK29" s="36" t="s">
         <v>818</v>
       </c>
-    </row>
-    <row r="30" spans="5:66" ht="30">
+      <c r="BL29" s="35"/>
+      <c r="BM29" s="35"/>
+      <c r="BN29" s="35"/>
+      <c r="BO29" s="35"/>
+      <c r="BP29" s="35"/>
+      <c r="BQ29" s="35"/>
+      <c r="BR29" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="BS29" s="36" t="s">
+        <v>656</v>
+      </c>
+      <c r="BT29" s="35"/>
+      <c r="BU29" s="35"/>
+      <c r="BV29" s="35"/>
+      <c r="BW29" s="35"/>
+      <c r="BX29" s="35"/>
+      <c r="BY29" s="35"/>
+      <c r="CN29" s="25" t="s">
+        <v>400</v>
+      </c>
+      <c r="CO29" s="25" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="30" spans="5:105" ht="31.5">
       <c r="O30" s="25" t="s">
         <v>39</v>
       </c>
@@ -13422,8 +14414,29 @@
       <c r="BH30" s="25" t="s">
         <v>958</v>
       </c>
-    </row>
-    <row r="31" spans="5:66" ht="30">
+      <c r="BI30" s="35"/>
+      <c r="BJ30" s="36" t="s">
+        <v>836</v>
+      </c>
+      <c r="BK30" s="36" t="s">
+        <v>837</v>
+      </c>
+      <c r="BL30" s="35"/>
+      <c r="BM30" s="35"/>
+      <c r="BN30" s="35"/>
+      <c r="BO30" s="35"/>
+      <c r="BP30" s="35"/>
+      <c r="BQ30" s="35"/>
+      <c r="BR30" s="35"/>
+      <c r="BS30" s="35"/>
+      <c r="BT30" s="35"/>
+      <c r="BU30" s="35"/>
+      <c r="BV30" s="35"/>
+      <c r="BW30" s="35"/>
+      <c r="BX30" s="35"/>
+      <c r="BY30" s="35"/>
+    </row>
+    <row r="31" spans="5:105" ht="31.5">
       <c r="O31" s="25" t="s">
         <v>40</v>
       </c>
@@ -13460,8 +14473,29 @@
       <c r="BH31" s="25" t="s">
         <v>959</v>
       </c>
-    </row>
-    <row r="32" spans="5:66" ht="30">
+      <c r="BI31" s="35"/>
+      <c r="BJ31" s="36" t="s">
+        <v>838</v>
+      </c>
+      <c r="BK31" s="36" t="s">
+        <v>839</v>
+      </c>
+      <c r="BL31" s="35"/>
+      <c r="BM31" s="35"/>
+      <c r="BN31" s="35"/>
+      <c r="BO31" s="35"/>
+      <c r="BP31" s="35"/>
+      <c r="BQ31" s="35"/>
+      <c r="BR31" s="35"/>
+      <c r="BS31" s="35"/>
+      <c r="BT31" s="35"/>
+      <c r="BU31" s="35"/>
+      <c r="BV31" s="35"/>
+      <c r="BW31" s="35"/>
+      <c r="BX31" s="35"/>
+      <c r="BY31" s="35"/>
+    </row>
+    <row r="32" spans="5:105" ht="31.5">
       <c r="O32" s="25" t="s">
         <v>36</v>
       </c>
@@ -13498,8 +14532,29 @@
       <c r="BH32" s="25" t="s">
         <v>960</v>
       </c>
-    </row>
-    <row r="33" spans="15:60" ht="30">
+      <c r="BI32" s="35"/>
+      <c r="BJ32" s="36" t="s">
+        <v>659</v>
+      </c>
+      <c r="BK32" s="36" t="s">
+        <v>660</v>
+      </c>
+      <c r="BL32" s="35"/>
+      <c r="BM32" s="35"/>
+      <c r="BN32" s="35"/>
+      <c r="BO32" s="35"/>
+      <c r="BP32" s="35"/>
+      <c r="BQ32" s="35"/>
+      <c r="BR32" s="35"/>
+      <c r="BS32" s="35"/>
+      <c r="BT32" s="35"/>
+      <c r="BU32" s="35"/>
+      <c r="BV32" s="35"/>
+      <c r="BW32" s="35"/>
+      <c r="BX32" s="35"/>
+      <c r="BY32" s="35"/>
+    </row>
+    <row r="33" spans="15:77" ht="31.5">
       <c r="O33" s="25" t="s">
         <v>33</v>
       </c>
@@ -13536,8 +14591,29 @@
       <c r="BH33" s="25" t="s">
         <v>961</v>
       </c>
-    </row>
-    <row r="34" spans="15:60" ht="30">
+      <c r="BI33" s="35"/>
+      <c r="BJ33" s="36" t="s">
+        <v>659</v>
+      </c>
+      <c r="BK33" s="36" t="s">
+        <v>661</v>
+      </c>
+      <c r="BL33" s="35"/>
+      <c r="BM33" s="35"/>
+      <c r="BN33" s="35"/>
+      <c r="BO33" s="35"/>
+      <c r="BP33" s="35"/>
+      <c r="BQ33" s="35"/>
+      <c r="BR33" s="35"/>
+      <c r="BS33" s="35"/>
+      <c r="BT33" s="35"/>
+      <c r="BU33" s="35"/>
+      <c r="BV33" s="35"/>
+      <c r="BW33" s="35"/>
+      <c r="BX33" s="35"/>
+      <c r="BY33" s="35"/>
+    </row>
+    <row r="34" spans="15:77" ht="30">
       <c r="O34" s="25" t="s">
         <v>170</v>
       </c>
@@ -13574,8 +14650,29 @@
       <c r="BH34" s="25" t="s">
         <v>962</v>
       </c>
-    </row>
-    <row r="35" spans="15:60" ht="30">
+      <c r="BI34" s="35"/>
+      <c r="BJ34" s="36" t="s">
+        <v>662</v>
+      </c>
+      <c r="BK34" s="36" t="s">
+        <v>663</v>
+      </c>
+      <c r="BL34" s="35"/>
+      <c r="BM34" s="35"/>
+      <c r="BN34" s="35"/>
+      <c r="BO34" s="35"/>
+      <c r="BP34" s="35"/>
+      <c r="BQ34" s="35"/>
+      <c r="BR34" s="35"/>
+      <c r="BS34" s="35"/>
+      <c r="BT34" s="35"/>
+      <c r="BU34" s="35"/>
+      <c r="BV34" s="35"/>
+      <c r="BW34" s="35"/>
+      <c r="BX34" s="35"/>
+      <c r="BY34" s="35"/>
+    </row>
+    <row r="35" spans="15:77" ht="31.5">
       <c r="O35" s="25" t="s">
         <v>86</v>
       </c>
@@ -13606,8 +14703,29 @@
       <c r="BH35" s="25" t="s">
         <v>963</v>
       </c>
-    </row>
-    <row r="36" spans="15:60" ht="30">
+      <c r="BI35" s="35"/>
+      <c r="BJ35" s="36" t="s">
+        <v>63</v>
+      </c>
+      <c r="BK35" s="36" t="s">
+        <v>664</v>
+      </c>
+      <c r="BL35" s="35"/>
+      <c r="BM35" s="35"/>
+      <c r="BN35" s="35"/>
+      <c r="BO35" s="35"/>
+      <c r="BP35" s="35"/>
+      <c r="BQ35" s="35"/>
+      <c r="BR35" s="35"/>
+      <c r="BS35" s="35"/>
+      <c r="BT35" s="35"/>
+      <c r="BU35" s="35"/>
+      <c r="BV35" s="35"/>
+      <c r="BW35" s="35"/>
+      <c r="BX35" s="35"/>
+      <c r="BY35" s="35"/>
+    </row>
+    <row r="36" spans="15:77" ht="30">
       <c r="O36" s="25" t="s">
         <v>48</v>
       </c>
@@ -13638,8 +14756,25 @@
       <c r="BH36" s="25" t="s">
         <v>964</v>
       </c>
-    </row>
-    <row r="37" spans="15:60" ht="30">
+      <c r="BI36" s="35"/>
+      <c r="BJ36" s="35"/>
+      <c r="BK36" s="35"/>
+      <c r="BL36" s="35"/>
+      <c r="BM36" s="35"/>
+      <c r="BN36" s="35"/>
+      <c r="BO36" s="35"/>
+      <c r="BP36" s="35"/>
+      <c r="BQ36" s="35"/>
+      <c r="BR36" s="35"/>
+      <c r="BS36" s="35"/>
+      <c r="BT36" s="35"/>
+      <c r="BU36" s="35"/>
+      <c r="BV36" s="35"/>
+      <c r="BW36" s="35"/>
+      <c r="BX36" s="35"/>
+      <c r="BY36" s="35"/>
+    </row>
+    <row r="37" spans="15:77" ht="30">
       <c r="O37" s="25" t="s">
         <v>87</v>
       </c>
@@ -13670,8 +14805,25 @@
       <c r="BH37" s="25" t="s">
         <v>965</v>
       </c>
-    </row>
-    <row r="38" spans="15:60">
+      <c r="BI37" s="35"/>
+      <c r="BJ37" s="35"/>
+      <c r="BK37" s="35"/>
+      <c r="BL37" s="35"/>
+      <c r="BM37" s="35"/>
+      <c r="BN37" s="35"/>
+      <c r="BO37" s="35"/>
+      <c r="BP37" s="35"/>
+      <c r="BQ37" s="35"/>
+      <c r="BR37" s="35"/>
+      <c r="BS37" s="35"/>
+      <c r="BT37" s="35"/>
+      <c r="BU37" s="35"/>
+      <c r="BV37" s="35"/>
+      <c r="BW37" s="35"/>
+      <c r="BX37" s="35"/>
+      <c r="BY37" s="35"/>
+    </row>
+    <row r="38" spans="15:77" ht="15.75">
       <c r="AU38" s="25" t="s">
         <v>722</v>
       </c>
@@ -13690,8 +14842,25 @@
       <c r="BH38" s="25" t="s">
         <v>966</v>
       </c>
-    </row>
-    <row r="39" spans="15:60">
+      <c r="BI38" s="35"/>
+      <c r="BJ38" s="35"/>
+      <c r="BK38" s="35"/>
+      <c r="BL38" s="35"/>
+      <c r="BM38" s="35"/>
+      <c r="BN38" s="35"/>
+      <c r="BO38" s="35"/>
+      <c r="BP38" s="35"/>
+      <c r="BQ38" s="35"/>
+      <c r="BR38" s="35"/>
+      <c r="BS38" s="35"/>
+      <c r="BT38" s="35"/>
+      <c r="BU38" s="35"/>
+      <c r="BV38" s="35"/>
+      <c r="BW38" s="35"/>
+      <c r="BX38" s="35"/>
+      <c r="BY38" s="35"/>
+    </row>
+    <row r="39" spans="15:77" ht="15.75">
       <c r="AU39" s="25" t="s">
         <v>722</v>
       </c>
@@ -13710,8 +14879,25 @@
       <c r="BH39" s="25" t="s">
         <v>967</v>
       </c>
-    </row>
-    <row r="40" spans="15:60">
+      <c r="BI39" s="35"/>
+      <c r="BJ39" s="35"/>
+      <c r="BK39" s="35"/>
+      <c r="BL39" s="35"/>
+      <c r="BM39" s="35"/>
+      <c r="BN39" s="35"/>
+      <c r="BO39" s="35"/>
+      <c r="BP39" s="35"/>
+      <c r="BQ39" s="35"/>
+      <c r="BR39" s="35"/>
+      <c r="BS39" s="35"/>
+      <c r="BT39" s="35"/>
+      <c r="BU39" s="35"/>
+      <c r="BV39" s="35"/>
+      <c r="BW39" s="35"/>
+      <c r="BX39" s="35"/>
+      <c r="BY39" s="35"/>
+    </row>
+    <row r="40" spans="15:77" ht="15.75">
       <c r="AU40" s="25" t="s">
         <v>722</v>
       </c>
@@ -13730,8 +14916,25 @@
       <c r="BH40" s="25" t="s">
         <v>968</v>
       </c>
-    </row>
-    <row r="41" spans="15:60">
+      <c r="BI40" s="35"/>
+      <c r="BJ40" s="35"/>
+      <c r="BK40" s="35"/>
+      <c r="BL40" s="35"/>
+      <c r="BM40" s="35"/>
+      <c r="BN40" s="35"/>
+      <c r="BO40" s="35"/>
+      <c r="BP40" s="35"/>
+      <c r="BQ40" s="35"/>
+      <c r="BR40" s="35"/>
+      <c r="BS40" s="35"/>
+      <c r="BT40" s="35"/>
+      <c r="BU40" s="35"/>
+      <c r="BV40" s="35"/>
+      <c r="BW40" s="35"/>
+      <c r="BX40" s="35"/>
+      <c r="BY40" s="35"/>
+    </row>
+    <row r="41" spans="15:77" ht="15.75">
       <c r="AU41" s="25" t="s">
         <v>722</v>
       </c>
@@ -13750,8 +14953,25 @@
       <c r="BH41" s="25" t="s">
         <v>969</v>
       </c>
-    </row>
-    <row r="42" spans="15:60">
+      <c r="BI41" s="35"/>
+      <c r="BJ41" s="35"/>
+      <c r="BK41" s="35"/>
+      <c r="BL41" s="35"/>
+      <c r="BM41" s="35"/>
+      <c r="BN41" s="35"/>
+      <c r="BO41" s="35"/>
+      <c r="BP41" s="35"/>
+      <c r="BQ41" s="35"/>
+      <c r="BR41" s="35"/>
+      <c r="BS41" s="35"/>
+      <c r="BT41" s="35"/>
+      <c r="BU41" s="35"/>
+      <c r="BV41" s="35"/>
+      <c r="BW41" s="35"/>
+      <c r="BX41" s="35"/>
+      <c r="BY41" s="35"/>
+    </row>
+    <row r="42" spans="15:77" ht="15.75">
       <c r="AU42" s="25" t="s">
         <v>722</v>
       </c>
@@ -13770,8 +14990,25 @@
       <c r="BH42" s="25" t="s">
         <v>970</v>
       </c>
-    </row>
-    <row r="43" spans="15:60">
+      <c r="BI42" s="35"/>
+      <c r="BJ42" s="35"/>
+      <c r="BK42" s="35"/>
+      <c r="BL42" s="35"/>
+      <c r="BM42" s="35"/>
+      <c r="BN42" s="35"/>
+      <c r="BO42" s="35"/>
+      <c r="BP42" s="35"/>
+      <c r="BQ42" s="35"/>
+      <c r="BR42" s="35"/>
+      <c r="BS42" s="35"/>
+      <c r="BT42" s="35"/>
+      <c r="BU42" s="35"/>
+      <c r="BV42" s="35"/>
+      <c r="BW42" s="35"/>
+      <c r="BX42" s="35"/>
+      <c r="BY42" s="35"/>
+    </row>
+    <row r="43" spans="15:77" ht="15.75">
       <c r="AU43" s="25" t="s">
         <v>722</v>
       </c>
@@ -13790,8 +15027,25 @@
       <c r="BH43" s="25" t="s">
         <v>971</v>
       </c>
-    </row>
-    <row r="44" spans="15:60">
+      <c r="BI43" s="35"/>
+      <c r="BJ43" s="35"/>
+      <c r="BK43" s="35"/>
+      <c r="BL43" s="35"/>
+      <c r="BM43" s="35"/>
+      <c r="BN43" s="35"/>
+      <c r="BO43" s="35"/>
+      <c r="BP43" s="35"/>
+      <c r="BQ43" s="35"/>
+      <c r="BR43" s="35"/>
+      <c r="BS43" s="35"/>
+      <c r="BT43" s="35"/>
+      <c r="BU43" s="35"/>
+      <c r="BV43" s="35"/>
+      <c r="BW43" s="35"/>
+      <c r="BX43" s="35"/>
+      <c r="BY43" s="35"/>
+    </row>
+    <row r="44" spans="15:77" ht="15.75">
       <c r="AU44" s="25" t="s">
         <v>722</v>
       </c>
@@ -13810,8 +15064,25 @@
       <c r="BH44" s="25" t="s">
         <v>972</v>
       </c>
-    </row>
-    <row r="45" spans="15:60">
+      <c r="BI44" s="35"/>
+      <c r="BJ44" s="35"/>
+      <c r="BK44" s="35"/>
+      <c r="BL44" s="35"/>
+      <c r="BM44" s="35"/>
+      <c r="BN44" s="35"/>
+      <c r="BO44" s="35"/>
+      <c r="BP44" s="35"/>
+      <c r="BQ44" s="35"/>
+      <c r="BR44" s="35"/>
+      <c r="BS44" s="35"/>
+      <c r="BT44" s="35"/>
+      <c r="BU44" s="35"/>
+      <c r="BV44" s="35"/>
+      <c r="BW44" s="35"/>
+      <c r="BX44" s="35"/>
+      <c r="BY44" s="35"/>
+    </row>
+    <row r="45" spans="15:77" ht="15.75">
       <c r="AU45" s="25" t="s">
         <v>722</v>
       </c>
@@ -13830,8 +15101,25 @@
       <c r="BH45" s="25" t="s">
         <v>973</v>
       </c>
-    </row>
-    <row r="46" spans="15:60">
+      <c r="BI45" s="35"/>
+      <c r="BJ45" s="35"/>
+      <c r="BK45" s="35"/>
+      <c r="BL45" s="35"/>
+      <c r="BM45" s="35"/>
+      <c r="BN45" s="35"/>
+      <c r="BO45" s="35"/>
+      <c r="BP45" s="35"/>
+      <c r="BQ45" s="35"/>
+      <c r="BR45" s="35"/>
+      <c r="BS45" s="35"/>
+      <c r="BT45" s="35"/>
+      <c r="BU45" s="35"/>
+      <c r="BV45" s="35"/>
+      <c r="BW45" s="35"/>
+      <c r="BX45" s="35"/>
+      <c r="BY45" s="35"/>
+    </row>
+    <row r="46" spans="15:77" ht="15.75">
       <c r="AU46" s="25" t="s">
         <v>722</v>
       </c>
@@ -13850,8 +15138,25 @@
       <c r="BH46" s="25" t="s">
         <v>974</v>
       </c>
-    </row>
-    <row r="47" spans="15:60">
+      <c r="BI46" s="35"/>
+      <c r="BJ46" s="35"/>
+      <c r="BK46" s="35"/>
+      <c r="BL46" s="35"/>
+      <c r="BM46" s="35"/>
+      <c r="BN46" s="35"/>
+      <c r="BO46" s="35"/>
+      <c r="BP46" s="35"/>
+      <c r="BQ46" s="35"/>
+      <c r="BR46" s="35"/>
+      <c r="BS46" s="35"/>
+      <c r="BT46" s="35"/>
+      <c r="BU46" s="35"/>
+      <c r="BV46" s="35"/>
+      <c r="BW46" s="35"/>
+      <c r="BX46" s="35"/>
+      <c r="BY46" s="35"/>
+    </row>
+    <row r="47" spans="15:77" ht="15.75">
       <c r="AU47" s="25" t="s">
         <v>722</v>
       </c>
@@ -13870,8 +15175,25 @@
       <c r="BH47" s="25" t="s">
         <v>975</v>
       </c>
-    </row>
-    <row r="48" spans="15:60">
+      <c r="BI47" s="35"/>
+      <c r="BJ47" s="35"/>
+      <c r="BK47" s="35"/>
+      <c r="BL47" s="35"/>
+      <c r="BM47" s="35"/>
+      <c r="BN47" s="35"/>
+      <c r="BO47" s="35"/>
+      <c r="BP47" s="35"/>
+      <c r="BQ47" s="35"/>
+      <c r="BR47" s="35"/>
+      <c r="BS47" s="35"/>
+      <c r="BT47" s="35"/>
+      <c r="BU47" s="35"/>
+      <c r="BV47" s="35"/>
+      <c r="BW47" s="35"/>
+      <c r="BX47" s="35"/>
+      <c r="BY47" s="35"/>
+    </row>
+    <row r="48" spans="15:77" ht="15.75">
       <c r="AU48" s="25" t="s">
         <v>722</v>
       </c>
@@ -13890,8 +15212,25 @@
       <c r="BH48" s="25" t="s">
         <v>976</v>
       </c>
-    </row>
-    <row r="49" spans="47:60">
+      <c r="BI48" s="35"/>
+      <c r="BJ48" s="35"/>
+      <c r="BK48" s="35"/>
+      <c r="BL48" s="35"/>
+      <c r="BM48" s="35"/>
+      <c r="BN48" s="35"/>
+      <c r="BO48" s="35"/>
+      <c r="BP48" s="35"/>
+      <c r="BQ48" s="35"/>
+      <c r="BR48" s="35"/>
+      <c r="BS48" s="35"/>
+      <c r="BT48" s="35"/>
+      <c r="BU48" s="35"/>
+      <c r="BV48" s="35"/>
+      <c r="BW48" s="35"/>
+      <c r="BX48" s="35"/>
+      <c r="BY48" s="35"/>
+    </row>
+    <row r="49" spans="47:77" ht="15.75">
       <c r="AU49" s="25" t="s">
         <v>722</v>
       </c>
@@ -13910,8 +15249,25 @@
       <c r="BH49" s="25" t="s">
         <v>977</v>
       </c>
-    </row>
-    <row r="50" spans="47:60">
+      <c r="BI49" s="35"/>
+      <c r="BJ49" s="35"/>
+      <c r="BK49" s="35"/>
+      <c r="BL49" s="35"/>
+      <c r="BM49" s="35"/>
+      <c r="BN49" s="35"/>
+      <c r="BO49" s="35"/>
+      <c r="BP49" s="35"/>
+      <c r="BQ49" s="35"/>
+      <c r="BR49" s="35"/>
+      <c r="BS49" s="35"/>
+      <c r="BT49" s="35"/>
+      <c r="BU49" s="35"/>
+      <c r="BV49" s="35"/>
+      <c r="BW49" s="35"/>
+      <c r="BX49" s="35"/>
+      <c r="BY49" s="35"/>
+    </row>
+    <row r="50" spans="47:77">
       <c r="AU50" s="25" t="s">
         <v>722</v>
       </c>
@@ -13931,7 +15287,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="51" spans="47:60">
+    <row r="51" spans="47:77">
       <c r="AU51" s="25" t="s">
         <v>722</v>
       </c>
@@ -13951,7 +15307,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="52" spans="47:60">
+    <row r="52" spans="47:77">
       <c r="BD52" s="25" t="s">
         <v>30</v>
       </c>
@@ -13965,7 +15321,7 @@
         <v>980</v>
       </c>
     </row>
-    <row r="53" spans="47:60">
+    <row r="53" spans="47:77">
       <c r="BD53" s="25" t="s">
         <v>30</v>
       </c>
@@ -13979,7 +15335,7 @@
         <v>981</v>
       </c>
     </row>
-    <row r="54" spans="47:60">
+    <row r="54" spans="47:77">
       <c r="BD54" s="25" t="s">
         <v>30</v>
       </c>
@@ -13993,7 +15349,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="55" spans="47:60">
+    <row r="55" spans="47:77">
       <c r="BD55" s="25" t="s">
         <v>30</v>
       </c>
@@ -14007,7 +15363,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="56" spans="47:60">
+    <row r="56" spans="47:77">
       <c r="BD56" s="25" t="s">
         <v>30</v>
       </c>
@@ -14021,7 +15377,7 @@
         <v>984</v>
       </c>
     </row>
-    <row r="57" spans="47:60">
+    <row r="57" spans="47:77">
       <c r="BD57" s="25" t="s">
         <v>30</v>
       </c>
@@ -14035,7 +15391,7 @@
         <v>985</v>
       </c>
     </row>
-    <row r="58" spans="47:60">
+    <row r="58" spans="47:77">
       <c r="BD58" s="25" t="s">
         <v>30</v>
       </c>
@@ -14049,7 +15405,7 @@
         <v>986</v>
       </c>
     </row>
-    <row r="59" spans="47:60">
+    <row r="59" spans="47:77">
       <c r="BD59" s="25" t="s">
         <v>30</v>
       </c>
@@ -14063,7 +15419,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="60" spans="47:60">
+    <row r="60" spans="47:77">
       <c r="BD60" s="25" t="s">
         <v>30</v>
       </c>
@@ -14077,7 +15433,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="61" spans="47:60">
+    <row r="61" spans="47:77">
       <c r="BD61" s="25" t="s">
         <v>30</v>
       </c>
@@ -14091,7 +15447,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="62" spans="47:60">
+    <row r="62" spans="47:77">
       <c r="BD62" s="25" t="s">
         <v>30</v>
       </c>
@@ -14105,7 +15461,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="63" spans="47:60">
+    <row r="63" spans="47:77">
       <c r="BD63" s="25" t="s">
         <v>30</v>
       </c>
@@ -14119,7 +15475,7 @@
         <v>991</v>
       </c>
     </row>
-    <row r="64" spans="47:60">
+    <row r="64" spans="47:77">
       <c r="BD64" s="25" t="s">
         <v>30</v>
       </c>

</xml_diff>

<commit_message>
Added LPC Interface and checked for repeat pins
</commit_message>
<xml_diff>
--- a/Excel Sheet/Southbridge.xlsx
+++ b/Excel Sheet/Southbridge.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4506"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="20520" windowHeight="11640" activeTab="2"/>
@@ -11,12 +11,12 @@
     <sheet name="signal list" sheetId="2" r:id="rId2"/>
     <sheet name="sorted list" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2975" uniqueCount="1072">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3051" uniqueCount="1078">
   <si>
     <t>A</t>
   </si>
@@ -3232,6 +3232,24 @@
   </si>
   <si>
     <t>Other</t>
+  </si>
+  <si>
+    <t>Firmware Hub Interface</t>
+  </si>
+  <si>
+    <t>FWH Signals</t>
+  </si>
+  <si>
+    <t>LPC Interface</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LOOK AT INTERSECTING PINS </t>
+  </si>
+  <si>
+    <t>Interrupt Interface</t>
+  </si>
+  <si>
+    <t>Processor Interface</t>
   </si>
 </sst>
 </file>
@@ -3483,7 +3501,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -3577,6 +3595,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -5809,8 +5828,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D677"/>
   <sheetViews>
-    <sheetView topLeftCell="A112" workbookViewId="0">
-      <selection activeCell="F121" sqref="F121"/>
+    <sheetView topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114:D114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5835,10 +5854,10 @@
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A3" s="9" t="s">
+      <c r="C3" s="9" t="s">
         <v>124</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="D3" s="10" t="s">
         <v>125</v>
       </c>
     </row>
@@ -6330,7 +6349,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="65" spans="1:4" ht="15.75" thickBot="1">
+    <row r="65" spans="3:4" ht="15.75" thickBot="1">
       <c r="C65" s="9" t="s">
         <v>229</v>
       </c>
@@ -6338,7 +6357,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="66" spans="1:4" ht="15.75" thickBot="1">
+    <row r="66" spans="3:4" ht="15.75" thickBot="1">
       <c r="C66" s="9" t="s">
         <v>231</v>
       </c>
@@ -6346,7 +6365,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="67" spans="1:4" ht="15.75" thickBot="1">
+    <row r="67" spans="3:4" ht="15.75" thickBot="1">
       <c r="C67" s="9" t="s">
         <v>233</v>
       </c>
@@ -6354,7 +6373,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="68" spans="1:4" ht="15.75" thickBot="1">
+    <row r="68" spans="3:4" ht="15.75" thickBot="1">
       <c r="C68" s="9" t="s">
         <v>235</v>
       </c>
@@ -6362,7 +6381,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="69" spans="1:4" ht="15.75" thickBot="1">
+    <row r="69" spans="3:4" ht="15.75" thickBot="1">
       <c r="C69" s="9" t="s">
         <v>236</v>
       </c>
@@ -6370,15 +6389,15 @@
         <v>48</v>
       </c>
     </row>
-    <row r="70" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A70" s="9" t="s">
+    <row r="70" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C70" s="9" t="s">
         <v>237</v>
       </c>
-      <c r="B70" s="10" t="s">
+      <c r="D70" s="10" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="71" spans="1:4" ht="15.75" thickBot="1">
+    <row r="71" spans="3:4" ht="15.75" thickBot="1">
       <c r="C71" s="9" t="s">
         <v>239</v>
       </c>
@@ -6386,47 +6405,47 @@
         <v>240</v>
       </c>
     </row>
-    <row r="72" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A72" s="7" t="s">
+    <row r="72" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C72" s="7" t="s">
         <v>241</v>
       </c>
-      <c r="B72" s="8" t="s">
+      <c r="D72" s="8" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="73" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A73" s="9" t="s">
+    <row r="73" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C73" s="9" t="s">
         <v>243</v>
       </c>
-      <c r="B73" s="10" t="s">
+      <c r="D73" s="10" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="74" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A74" s="9" t="s">
+    <row r="74" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C74" s="9" t="s">
         <v>245</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="D74" s="10" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="75" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A75" s="9" t="s">
+    <row r="75" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C75" s="9" t="s">
         <v>247</v>
       </c>
-      <c r="B75" s="10" t="s">
+      <c r="D75" s="10" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="76" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A76" s="9" t="s">
+    <row r="76" spans="3:4" ht="21.75" thickBot="1">
+      <c r="C76" s="9" t="s">
         <v>249</v>
       </c>
-      <c r="B76" s="10" t="s">
+      <c r="D76" s="10" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="77" spans="1:4" ht="21.75" thickBot="1">
+    <row r="77" spans="3:4" ht="21.75" thickBot="1">
       <c r="C77" s="9" t="s">
         <v>251</v>
       </c>
@@ -6434,7 +6453,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="78" spans="1:4" ht="21.75" thickBot="1">
+    <row r="78" spans="3:4" ht="21.75" thickBot="1">
       <c r="C78" s="9" t="s">
         <v>253</v>
       </c>
@@ -6442,7 +6461,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="79" spans="1:4" ht="21.75" thickBot="1">
+    <row r="79" spans="3:4" ht="21.75" thickBot="1">
       <c r="C79" s="9" t="s">
         <v>255</v>
       </c>
@@ -6450,7 +6469,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="80" spans="1:4" ht="15.75" thickBot="1">
+    <row r="80" spans="3:4" ht="15.75" thickBot="1">
       <c r="C80" s="7" t="s">
         <v>106</v>
       </c>
@@ -6699,34 +6718,34 @@
       </c>
     </row>
     <row r="111" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A111" s="9" t="s">
+      <c r="C111" s="9" t="s">
         <v>308</v>
       </c>
-      <c r="B111" s="10" t="s">
+      <c r="D111" s="10" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="112" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A112" s="9" t="s">
+      <c r="C112" s="9" t="s">
         <v>310</v>
       </c>
-      <c r="B112" s="10" t="s">
+      <c r="D112" s="10" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A113" s="9" t="s">
+    <row r="113" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C113" s="9" t="s">
         <v>91</v>
       </c>
-      <c r="B113" s="10" t="s">
+      <c r="D113" s="10" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="114" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A114" s="9" t="s">
+      <c r="C114" s="9" t="s">
         <v>313</v>
       </c>
-      <c r="B114" s="10" t="s">
+      <c r="D114" s="10" t="s">
         <v>314</v>
       </c>
     </row>
@@ -7098,7 +7117,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="161" spans="1:4" ht="15.75" thickBot="1">
+    <row r="161" spans="3:4" ht="15.75" thickBot="1">
       <c r="C161" s="9" t="s">
         <v>403</v>
       </c>
@@ -7106,7 +7125,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="162" spans="1:4" ht="15.75" thickBot="1">
+    <row r="162" spans="3:4" ht="15.75" thickBot="1">
       <c r="C162" s="9" t="s">
         <v>405</v>
       </c>
@@ -7114,7 +7133,7 @@
         <v>406</v>
       </c>
     </row>
-    <row r="163" spans="1:4" ht="15.75" thickBot="1">
+    <row r="163" spans="3:4" ht="15.75" thickBot="1">
       <c r="C163" s="9" t="s">
         <v>407</v>
       </c>
@@ -7122,7 +7141,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="164" spans="1:4" ht="15.75" thickBot="1">
+    <row r="164" spans="3:4" ht="15.75" thickBot="1">
       <c r="C164" s="9" t="s">
         <v>409</v>
       </c>
@@ -7130,7 +7149,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="165" spans="1:4" ht="15.75" thickBot="1">
+    <row r="165" spans="3:4" ht="15.75" thickBot="1">
       <c r="C165" s="9" t="s">
         <v>411</v>
       </c>
@@ -7138,7 +7157,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="166" spans="1:4" ht="21.75" thickBot="1">
+    <row r="166" spans="3:4" ht="21.75" thickBot="1">
       <c r="C166" s="9" t="s">
         <v>413</v>
       </c>
@@ -7146,7 +7165,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="167" spans="1:4" ht="15.75" thickBot="1">
+    <row r="167" spans="3:4" ht="15.75" thickBot="1">
       <c r="C167" s="9" t="s">
         <v>415</v>
       </c>
@@ -7154,7 +7173,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="168" spans="1:4" ht="15.75" thickBot="1">
+    <row r="168" spans="3:4" ht="15.75" thickBot="1">
       <c r="C168" s="9" t="s">
         <v>417</v>
       </c>
@@ -7162,7 +7181,7 @@
         <v>418</v>
       </c>
     </row>
-    <row r="169" spans="1:4" ht="15.75" thickBot="1">
+    <row r="169" spans="3:4" ht="15.75" thickBot="1">
       <c r="C169" s="9" t="s">
         <v>419</v>
       </c>
@@ -7170,7 +7189,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="170" spans="1:4" ht="15.75" thickBot="1">
+    <row r="170" spans="3:4" ht="15.75" thickBot="1">
       <c r="C170" s="9" t="s">
         <v>421</v>
       </c>
@@ -7178,7 +7197,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="171" spans="1:4" ht="15.75" thickBot="1">
+    <row r="171" spans="3:4" ht="15.75" thickBot="1">
       <c r="C171" s="9" t="s">
         <v>423</v>
       </c>
@@ -7186,7 +7205,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="172" spans="1:4" ht="21.75" thickBot="1">
+    <row r="172" spans="3:4" ht="21.75" thickBot="1">
       <c r="C172" s="9" t="s">
         <v>425</v>
       </c>
@@ -7194,67 +7213,67 @@
         <v>426</v>
       </c>
     </row>
-    <row r="173" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A173" s="9" t="s">
+    <row r="173" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C173" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="B173" s="10" t="s">
+      <c r="D173" s="10" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="174" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A174" s="9" t="s">
+    <row r="174" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C174" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="B174" s="10" t="s">
+      <c r="D174" s="10" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="175" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A175" s="9" t="s">
+    <row r="175" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C175" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="B175" s="10" t="s">
+      <c r="D175" s="10" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="176" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A176" s="9" t="s">
+    <row r="176" spans="3:4" ht="15.75" thickBot="1">
+      <c r="C176" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="B176" s="10" t="s">
+      <c r="D176" s="10" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="177" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A177" s="9" t="s">
+    <row r="177" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C177" s="9" t="s">
         <v>431</v>
       </c>
-      <c r="B177" s="10" t="s">
+      <c r="D177" s="10" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="178" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A178" s="9" t="s">
+    <row r="178" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C178" s="9" t="s">
         <v>433</v>
       </c>
-      <c r="B178" s="10" t="s">
+      <c r="D178" s="10" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="179" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A179" s="9" t="s">
+    <row r="179" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C179" s="9" t="s">
         <v>435</v>
       </c>
-      <c r="B179" s="10" t="s">
+      <c r="D179" s="10" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="180" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A180" s="9" t="s">
+    <row r="180" spans="1:4" ht="21.75" thickBot="1">
+      <c r="C180" s="9" t="s">
         <v>437</v>
       </c>
-      <c r="B180" s="10" t="s">
+      <c r="D180" s="10" t="s">
         <v>438</v>
       </c>
     </row>
@@ -11242,10 +11261,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:DA106"/>
+  <dimension ref="B2:EK106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="CW14" sqref="CW14"/>
+    <sheetView tabSelected="1" topLeftCell="DP1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="ED13" sqref="ED13:EE13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -11281,7 +11300,7 @@
     <col min="71" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:105" ht="23.25">
+    <row r="2" spans="2:141" ht="23.25">
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
       <c r="D2" s="26"/>
@@ -11398,8 +11417,45 @@
       <c r="CX2" s="26"/>
       <c r="CY2" s="26"/>
       <c r="CZ2" s="26"/>
-    </row>
-    <row r="4" spans="2:105" ht="18.75">
+      <c r="DC2" s="26"/>
+      <c r="DD2" s="26" t="s">
+        <v>1072</v>
+      </c>
+      <c r="DE2" s="26"/>
+      <c r="DF2" s="26"/>
+      <c r="DG2" s="26"/>
+      <c r="DJ2" s="26"/>
+      <c r="DK2" s="26"/>
+      <c r="DL2" s="26"/>
+      <c r="DM2" s="26" t="s">
+        <v>1074</v>
+      </c>
+      <c r="DN2" s="26"/>
+      <c r="DO2" s="26"/>
+      <c r="DP2" s="26"/>
+      <c r="DQ2" s="26"/>
+      <c r="DT2" s="26"/>
+      <c r="DU2" s="26"/>
+      <c r="DV2" s="26"/>
+      <c r="DW2" s="26" t="s">
+        <v>1076</v>
+      </c>
+      <c r="DX2" s="26"/>
+      <c r="DY2" s="26"/>
+      <c r="DZ2" s="26"/>
+      <c r="EA2" s="26"/>
+      <c r="ED2" s="26"/>
+      <c r="EE2" s="26"/>
+      <c r="EF2" s="26"/>
+      <c r="EG2" s="26" t="s">
+        <v>1077</v>
+      </c>
+      <c r="EH2" s="26"/>
+      <c r="EI2" s="26"/>
+      <c r="EJ2" s="26"/>
+      <c r="EK2" s="26"/>
+    </row>
+    <row r="4" spans="2:141" ht="18.75">
       <c r="B4" s="23" t="s">
         <v>1044</v>
       </c>
@@ -11468,8 +11524,41 @@
         <v>1068</v>
       </c>
       <c r="CY4" s="23"/>
-    </row>
-    <row r="5" spans="2:105">
+      <c r="DC4" s="23" t="s">
+        <v>1073</v>
+      </c>
+      <c r="DF4" s="23" t="s">
+        <v>1065</v>
+      </c>
+      <c r="DJ4" s="23" t="s">
+        <v>1063</v>
+      </c>
+      <c r="DM4" s="23" t="s">
+        <v>1065</v>
+      </c>
+      <c r="DP4" s="23" t="s">
+        <v>1064</v>
+      </c>
+      <c r="DT4" s="23" t="s">
+        <v>1063</v>
+      </c>
+      <c r="DW4" s="23" t="s">
+        <v>1065</v>
+      </c>
+      <c r="DZ4" s="23" t="s">
+        <v>1064</v>
+      </c>
+      <c r="ED4" s="23" t="s">
+        <v>1063</v>
+      </c>
+      <c r="EG4" s="23" t="s">
+        <v>1065</v>
+      </c>
+      <c r="EJ4" s="23" t="s">
+        <v>1064</v>
+      </c>
+    </row>
+    <row r="5" spans="2:141">
       <c r="B5" s="22" t="s">
         <v>120</v>
       </c>
@@ -11647,8 +11736,75 @@
       </c>
       <c r="CY5" s="22"/>
       <c r="CZ5" s="22"/>
-    </row>
-    <row r="6" spans="2:105" ht="34.5" customHeight="1">
+      <c r="DC5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="DD5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="DF5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="DG5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="DI5" s="22"/>
+      <c r="DJ5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="DK5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="DM5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="DN5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="DP5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="DQ5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="DT5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="DU5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="DW5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="DX5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="DZ5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="EA5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="ED5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="EE5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="EG5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="EH5" s="22" t="s">
+        <v>121</v>
+      </c>
+      <c r="EJ5" s="22" t="s">
+        <v>120</v>
+      </c>
+      <c r="EK5" s="22" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="2:141" ht="34.5" customHeight="1">
       <c r="B6" s="25" t="s">
         <v>478</v>
       </c>
@@ -11826,8 +11982,20 @@
       <c r="CW6" s="25" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="7" spans="2:105" ht="18.75" customHeight="1">
+      <c r="DC6" s="25" t="s">
+        <v>241</v>
+      </c>
+      <c r="DD6" s="25" t="s">
+        <v>242</v>
+      </c>
+      <c r="DF6" s="25" t="s">
+        <v>91</v>
+      </c>
+      <c r="DG6" s="25" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="7" spans="2:141" ht="18.75" customHeight="1">
       <c r="B7" s="25" t="s">
         <v>488</v>
       </c>
@@ -12005,8 +12173,17 @@
       <c r="CW7" s="25" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="8" spans="2:105" ht="18.75" customHeight="1">
+      <c r="DC7" s="25" t="s">
+        <v>243</v>
+      </c>
+      <c r="DD7" s="25" t="s">
+        <v>244</v>
+      </c>
+      <c r="DJ7" s="37" t="s">
+        <v>1075</v>
+      </c>
+    </row>
+    <row r="8" spans="2:141" ht="18.75" customHeight="1">
       <c r="B8" s="25" t="s">
         <v>539</v>
       </c>
@@ -12165,8 +12342,14 @@
       <c r="CO8" s="25" t="s">
         <v>408</v>
       </c>
-    </row>
-    <row r="9" spans="2:105" ht="20.25" customHeight="1">
+      <c r="DC8" s="25" t="s">
+        <v>245</v>
+      </c>
+      <c r="DD8" s="25" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="9" spans="2:141" ht="20.25" customHeight="1" thickBot="1">
       <c r="B9" s="25" t="s">
         <v>541</v>
       </c>
@@ -12324,8 +12507,26 @@
       <c r="CO9" s="25" t="s">
         <v>410</v>
       </c>
-    </row>
-    <row r="10" spans="2:105" ht="31.5">
+      <c r="DC9" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="DD9" s="25" t="s">
+        <v>248</v>
+      </c>
+      <c r="DT9" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="DU9" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="ED9" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="EE9" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="2:141" ht="32.25" thickBot="1">
       <c r="B10" s="25" t="s">
         <v>543</v>
       </c>
@@ -12473,8 +12674,26 @@
       <c r="CO10" s="25" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="11" spans="2:105" ht="20.25" customHeight="1">
+      <c r="DC10" s="25" t="s">
+        <v>249</v>
+      </c>
+      <c r="DD10" s="25" t="s">
+        <v>250</v>
+      </c>
+      <c r="DT10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="DU10" s="10" t="s">
+        <v>428</v>
+      </c>
+      <c r="ED10" s="9" t="s">
+        <v>237</v>
+      </c>
+      <c r="EE10" s="10" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="2:141" ht="20.25" customHeight="1" thickBot="1">
       <c r="B11" s="25" t="s">
         <v>547</v>
       </c>
@@ -12622,8 +12841,20 @@
       <c r="CO11" s="25" t="s">
         <v>414</v>
       </c>
-    </row>
-    <row r="12" spans="2:105" ht="18" customHeight="1">
+      <c r="DT11" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="DU11" s="10" t="s">
+        <v>429</v>
+      </c>
+      <c r="ED11" s="9" t="s">
+        <v>308</v>
+      </c>
+      <c r="EE11" s="10" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="12" spans="2:141" ht="18" customHeight="1" thickBot="1">
       <c r="B12" s="25" t="s">
         <v>549</v>
       </c>
@@ -12765,8 +12996,20 @@
       <c r="CO12" s="25" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="13" spans="2:105" ht="31.5">
+      <c r="DT12" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="DU12" s="10" t="s">
+        <v>430</v>
+      </c>
+      <c r="ED12" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="EE12" s="10" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="13" spans="2:141" ht="32.25" thickBot="1">
       <c r="B13" s="25" t="s">
         <v>553</v>
       </c>
@@ -12902,8 +13145,20 @@
       <c r="CO13" s="25" t="s">
         <v>418</v>
       </c>
-    </row>
-    <row r="14" spans="2:105" ht="31.5">
+      <c r="DT13" s="9" t="s">
+        <v>431</v>
+      </c>
+      <c r="DU13" s="10" t="s">
+        <v>432</v>
+      </c>
+      <c r="ED13" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="EE13" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="14" spans="2:141" ht="32.25" thickBot="1">
       <c r="E14" s="25" t="s">
         <v>520</v>
       </c>
@@ -13035,8 +13290,14 @@
       </c>
       <c r="CZ14" s="34"/>
       <c r="DA14" s="34"/>
-    </row>
-    <row r="15" spans="2:105" ht="45">
+      <c r="DT14" s="9" t="s">
+        <v>433</v>
+      </c>
+      <c r="DU14" s="10" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="15" spans="2:141" ht="45.75" thickBot="1">
       <c r="E15" s="25" t="s">
         <v>522</v>
       </c>
@@ -13160,8 +13421,14 @@
       </c>
       <c r="CZ15" s="34"/>
       <c r="DA15" s="34"/>
-    </row>
-    <row r="16" spans="2:105" ht="31.5">
+      <c r="DT15" s="9" t="s">
+        <v>435</v>
+      </c>
+      <c r="DU15" s="10" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="16" spans="2:141" ht="32.25" thickBot="1">
       <c r="E16" s="25" t="s">
         <v>524</v>
       </c>
@@ -13281,6 +13548,12 @@
       </c>
       <c r="CZ16" s="34"/>
       <c r="DA16" s="34"/>
+      <c r="DT16" s="9" t="s">
+        <v>437</v>
+      </c>
+      <c r="DU16" s="10" t="s">
+        <v>438</v>
+      </c>
     </row>
     <row r="17" spans="5:105" ht="31.5">
       <c r="E17" s="25" t="s">

</xml_diff>